<commit_message>
Added NN041304 to Excel
</commit_message>
<xml_diff>
--- a/Models/TrainingError.xlsx
+++ b/Models/TrainingError.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackie\Desktop\ImgSegNN\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9585745-71C5-4CDC-95FD-7FDEB340C84D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59791B09-9387-48B3-9516-C2A3FDEA5264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3828,102 +3828,6 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>1.2137800000000001</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1.21323</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1.21268</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1.21211</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>1.21153</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1.2109300000000001</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1.2103200000000001</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1.2097100000000001</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1.2090799999999999</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1.20844</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1.2077800000000001</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1.20712</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1.2064600000000001</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>1.2057800000000001</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1.2051000000000001</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1.20444</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1.20377</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1.2031000000000001</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1.20242</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1.20174</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>1.2010400000000001</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1.20034</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1.19964</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>1.1989399999999999</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>1.19825</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>1.19756</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>1.1968700000000001</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>1.1961900000000001</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>1.1955199999999999</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>1.19486</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1.1941999999999999</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>1.19356</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1.19292</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7028,16 +6932,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>62864</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>169544</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7330,8 +7234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E513"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7372,6 +7276,9 @@
       <c r="D2">
         <v>1.4550799999999999</v>
       </c>
+      <c r="E2">
+        <v>2.5937199999999998</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -7386,6 +7293,9 @@
       <c r="D3">
         <v>1.2123200000000001</v>
       </c>
+      <c r="E3">
+        <v>1.367</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
@@ -7400,6 +7310,9 @@
       <c r="D4">
         <v>1.18127</v>
       </c>
+      <c r="E4">
+        <v>1.3120700000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -7414,6 +7327,9 @@
       <c r="D5">
         <v>1.1647700000000001</v>
       </c>
+      <c r="E5">
+        <v>1.2888500000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
@@ -7428,6 +7344,9 @@
       <c r="D6">
         <v>1.1539299999999999</v>
       </c>
+      <c r="E6">
+        <v>1.2759400000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
@@ -7442,6 +7361,9 @@
       <c r="D7">
         <v>1.14429</v>
       </c>
+      <c r="E7">
+        <v>1.26766</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
@@ -7456,6 +7378,9 @@
       <c r="D8">
         <v>1.13487</v>
       </c>
+      <c r="E8">
+        <v>1.26203</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
@@ -7470,6 +7395,9 @@
       <c r="D9">
         <v>1.1251800000000001</v>
       </c>
+      <c r="E9">
+        <v>1.2579800000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
@@ -7484,6 +7412,9 @@
       <c r="D10">
         <v>1.1159300000000001</v>
       </c>
+      <c r="E10">
+        <v>1.2549699999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
@@ -7498,6 +7429,9 @@
       <c r="D11">
         <v>1.1063099999999999</v>
       </c>
+      <c r="E11">
+        <v>1.2526200000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -7512,6 +7446,9 @@
       <c r="D12">
         <v>1.0964100000000001</v>
       </c>
+      <c r="E12">
+        <v>1.2507200000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
@@ -7526,6 +7463,9 @@
       <c r="D13">
         <v>1.0862099999999999</v>
       </c>
+      <c r="E13">
+        <v>1.24912</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
@@ -7540,6 +7480,9 @@
       <c r="D14">
         <v>1.0748800000000001</v>
       </c>
+      <c r="E14">
+        <v>1.2477400000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
@@ -7554,6 +7497,9 @@
       <c r="D15">
         <v>1.06287</v>
       </c>
+      <c r="E15">
+        <v>1.2464900000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
@@ -7568,8 +7514,11 @@
       <c r="D16">
         <v>1.0519000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>1.2454000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>1.0970599999999999</v>
       </c>
@@ -7582,8 +7531,11 @@
       <c r="D17">
         <v>1.0408599999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>1.2443599999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>1.09259</v>
       </c>
@@ -7596,8 +7548,11 @@
       <c r="D18">
         <v>1.03006</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>1.2433700000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>1.0862099999999999</v>
       </c>
@@ -7610,8 +7565,11 @@
       <c r="D19">
         <v>1.0193300000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>1.2423299999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>1.0807500000000001</v>
       </c>
@@ -7624,8 +7582,11 @@
       <c r="D20">
         <v>1.0099499999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>1.24129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>1.0752299999999999</v>
       </c>
@@ -7638,8 +7599,11 @@
       <c r="D21">
         <v>0.99824999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>1.24031</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>1.06873</v>
       </c>
@@ -7652,8 +7616,11 @@
       <c r="D22">
         <v>0.98738000000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>1.2394400000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>1.0640000000000001</v>
       </c>
@@ -7666,8 +7633,11 @@
       <c r="D23">
         <v>0.97380999999999995</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>1.23861</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>1.05697</v>
       </c>
@@ -7680,8 +7650,11 @@
       <c r="D24">
         <v>0.95870999999999995</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>1.23783</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>1.0506</v>
       </c>
@@ -7694,8 +7667,11 @@
       <c r="D25">
         <v>0.94657000000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>1.2370699999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>1.0446500000000001</v>
       </c>
@@ -7708,8 +7684,11 @@
       <c r="D26">
         <v>0.92986000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>1.2363299999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>1.0374099999999999</v>
       </c>
@@ -7722,8 +7701,11 @@
       <c r="D27">
         <v>0.91842999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>1.2356199999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>1.0299199999999999</v>
       </c>
@@ -7736,8 +7718,11 @@
       <c r="D28">
         <v>0.90283999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>1.2349300000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>1.02234</v>
       </c>
@@ -7750,8 +7735,11 @@
       <c r="D29">
         <v>0.89232999999999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>1.2342299999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>1.0116099999999999</v>
       </c>
@@ -7764,8 +7752,11 @@
       <c r="D30">
         <v>0.88227999999999995</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>1.2335199999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>1.00186</v>
       </c>
@@ -7778,8 +7769,11 @@
       <c r="D31">
         <v>0.86517999999999995</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>1.2327900000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>0.99263000000000001</v>
       </c>
@@ -7792,8 +7786,11 @@
       <c r="D32">
         <v>0.85448000000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>1.23201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>0.98448999999999998</v>
       </c>
@@ -7806,8 +7803,11 @@
       <c r="D33">
         <v>0.83909999999999996</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>1.2313000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>0.97646999999999995</v>
       </c>
@@ -7820,8 +7820,11 @@
       <c r="D34">
         <v>0.82679999999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>1.23064</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>0.96584000000000003</v>
       </c>
@@ -7834,8 +7837,11 @@
       <c r="D35">
         <v>0.81405000000000005</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>1.23001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>0.95508000000000004</v>
       </c>
@@ -7848,8 +7854,11 @@
       <c r="D36">
         <v>0.80705000000000005</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>1.22939</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>0.94486999999999999</v>
       </c>
@@ -7862,8 +7871,11 @@
       <c r="D37">
         <v>0.79708000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>1.2287999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>0.93822000000000005</v>
       </c>
@@ -7876,8 +7888,11 @@
       <c r="D38">
         <v>0.78922000000000003</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>1.2282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>0.92762999999999995</v>
       </c>
@@ -7890,8 +7905,11 @@
       <c r="D39">
         <v>0.77366999999999997</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>1.2276100000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>0.92034000000000005</v>
       </c>
@@ -7904,8 +7922,11 @@
       <c r="D40">
         <v>0.76861999999999997</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>1.22702</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>0.91352</v>
       </c>
@@ -7918,8 +7939,11 @@
       <c r="D41">
         <v>0.75548000000000004</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>1.22644</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>0.90368999999999999</v>
       </c>
@@ -7932,8 +7956,11 @@
       <c r="D42">
         <v>0.74595</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42">
+        <v>1.2258599999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>0.89685000000000004</v>
       </c>
@@ -7946,8 +7973,11 @@
       <c r="D43">
         <v>0.73960000000000004</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <v>1.22529</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>0.89124000000000003</v>
       </c>
@@ -7960,8 +7990,11 @@
       <c r="D44">
         <v>0.73185</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44">
+        <v>1.2247300000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>0.88793</v>
       </c>
@@ -7974,8 +8007,11 @@
       <c r="D45">
         <v>0.72047000000000005</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45">
+        <v>1.2241500000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>0.87975000000000003</v>
       </c>
@@ -7988,8 +8024,11 @@
       <c r="D46">
         <v>0.71225000000000005</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46">
+        <v>1.22357</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>0.87073</v>
       </c>
@@ -8002,8 +8041,11 @@
       <c r="D47">
         <v>0.71186000000000005</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47">
+        <v>1.2230099999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>0.86189000000000004</v>
       </c>
@@ -8016,8 +8058,11 @@
       <c r="D48">
         <v>0.69811999999999996</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48">
+        <v>1.22244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>0.85167000000000004</v>
       </c>
@@ -8030,8 +8075,11 @@
       <c r="D49">
         <v>0.69357999999999997</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49">
+        <v>1.2219</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>0.84370000000000001</v>
       </c>
@@ -8044,8 +8092,11 @@
       <c r="D50">
         <v>0.69576000000000005</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50">
+        <v>1.2213700000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>0.83496000000000004</v>
       </c>
@@ -8058,8 +8109,11 @@
       <c r="D51">
         <v>0.68600000000000005</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51">
+        <v>1.2208399999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>0.82221999999999995</v>
       </c>
@@ -8072,8 +8126,11 @@
       <c r="D52">
         <v>0.67688000000000004</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <v>1.2203200000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>0.81574000000000002</v>
       </c>
@@ -8086,8 +8143,11 @@
       <c r="D53">
         <v>0.66454000000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <v>1.2198100000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>0.80500000000000005</v>
       </c>
@@ -8100,8 +8160,11 @@
       <c r="D54">
         <v>0.65758000000000005</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <v>1.2193000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>0.79525000000000001</v>
       </c>
@@ -8114,8 +8177,11 @@
       <c r="D55">
         <v>0.64153000000000004</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55">
+        <v>1.2188099999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>0.78539000000000003</v>
       </c>
@@ -8128,8 +8194,11 @@
       <c r="D56">
         <v>0.63280999999999998</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56">
+        <v>1.2183200000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>0.78113999999999995</v>
       </c>
@@ -8142,8 +8211,11 @@
       <c r="D57">
         <v>0.62158999999999998</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57">
+        <v>1.21783</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>0.78739000000000003</v>
       </c>
@@ -8156,8 +8228,11 @@
       <c r="D58">
         <v>0.61992999999999998</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58">
+        <v>1.2173400000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>0.77329000000000003</v>
       </c>
@@ -8170,8 +8245,11 @@
       <c r="D59">
         <v>0.62409000000000003</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59">
+        <v>1.21685</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>0.76321000000000006</v>
       </c>
@@ -8184,8 +8262,11 @@
       <c r="D60">
         <v>0.61355999999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60">
+        <v>1.21635</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>0.75377000000000005</v>
       </c>
@@ -8198,8 +8279,11 @@
       <c r="D61">
         <v>0.60026000000000002</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61">
+        <v>1.2158599999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>0.75034999999999996</v>
       </c>
@@ -8212,8 +8296,11 @@
       <c r="D62">
         <v>0.59309000000000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62">
+        <v>1.2153499999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>0.74243000000000003</v>
       </c>
@@ -8226,8 +8313,11 @@
       <c r="D63">
         <v>0.59869000000000006</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63">
+        <v>1.2148399999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>0.73775000000000002</v>
       </c>
@@ -8240,8 +8330,11 @@
       <c r="D64">
         <v>0.5927</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64">
+        <v>1.2143200000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>0.72572000000000003</v>
       </c>
@@ -8254,456 +8347,459 @@
       <c r="D65">
         <v>0.58945999999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65">
+        <v>1.2137800000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>0.71723999999999999</v>
       </c>
-      <c r="B66">
-        <v>1.21323</v>
-      </c>
       <c r="C66">
         <v>0.55001</v>
       </c>
       <c r="D66">
         <v>0.58147000000000004</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66">
+        <v>1.21323</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>0.71008000000000004</v>
       </c>
-      <c r="B67">
-        <v>1.21268</v>
-      </c>
       <c r="C67">
         <v>0.55661000000000005</v>
       </c>
       <c r="D67">
         <v>0.56920999999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67">
+        <v>1.21268</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>0.71574000000000004</v>
       </c>
-      <c r="B68">
-        <v>1.21211</v>
-      </c>
       <c r="C68">
         <v>0.54752999999999996</v>
       </c>
       <c r="D68">
         <v>0.54952999999999996</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68">
+        <v>1.21211</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>0.69894999999999996</v>
       </c>
-      <c r="B69">
-        <v>1.21153</v>
-      </c>
       <c r="C69">
         <v>0.54742000000000002</v>
       </c>
       <c r="D69">
         <v>0.55583000000000005</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69">
+        <v>1.21153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>0.68415000000000004</v>
       </c>
-      <c r="B70">
-        <v>1.2109300000000001</v>
-      </c>
       <c r="C70">
         <v>0.54034000000000004</v>
       </c>
       <c r="D70">
         <v>0.53515999999999997</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70">
+        <v>1.2109300000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>0.67340999999999995</v>
       </c>
-      <c r="B71">
-        <v>1.2103200000000001</v>
-      </c>
       <c r="C71">
         <v>0.52003999999999995</v>
       </c>
       <c r="D71">
         <v>0.52797000000000005</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71">
+        <v>1.2103200000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>0.66666999999999998</v>
       </c>
-      <c r="B72">
-        <v>1.2097100000000001</v>
-      </c>
       <c r="C72">
         <v>0.50936999999999999</v>
       </c>
       <c r="D72">
         <v>0.51866999999999996</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72">
+        <v>1.2097100000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>0.66208</v>
       </c>
-      <c r="B73">
-        <v>1.2090799999999999</v>
-      </c>
       <c r="C73">
         <v>0.49428</v>
       </c>
       <c r="D73">
         <v>0.51670000000000005</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73">
+        <v>1.2090799999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>0.66693999999999998</v>
       </c>
-      <c r="B74">
-        <v>1.20844</v>
-      </c>
       <c r="C74">
         <v>0.48464000000000002</v>
       </c>
       <c r="D74">
         <v>0.51124999999999998</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74">
+        <v>1.20844</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>0.67162999999999995</v>
       </c>
-      <c r="B75">
-        <v>1.2077800000000001</v>
-      </c>
       <c r="C75">
         <v>0.48442000000000002</v>
       </c>
       <c r="D75">
         <v>0.50865000000000005</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75">
+        <v>1.2077800000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>0.65447999999999995</v>
       </c>
-      <c r="B76">
-        <v>1.20712</v>
-      </c>
       <c r="C76">
         <v>0.48116999999999999</v>
       </c>
       <c r="D76">
         <v>0.51075000000000004</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76">
+        <v>1.20712</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>0.64273999999999998</v>
       </c>
-      <c r="B77">
-        <v>1.2064600000000001</v>
-      </c>
       <c r="C77">
         <v>0.46965000000000001</v>
       </c>
       <c r="D77">
         <v>0.49995000000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77">
+        <v>1.2064600000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>0.64258999999999999</v>
       </c>
-      <c r="B78">
-        <v>1.2057800000000001</v>
-      </c>
       <c r="C78">
         <v>0.46010000000000001</v>
       </c>
       <c r="D78">
         <v>0.49647000000000002</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78">
+        <v>1.2057800000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>0.63590999999999998</v>
       </c>
-      <c r="B79">
-        <v>1.2051000000000001</v>
-      </c>
       <c r="C79">
         <v>0.45423999999999998</v>
       </c>
       <c r="D79">
         <v>0.48866999999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79">
+        <v>1.2051000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>0.62336000000000003</v>
       </c>
-      <c r="B80">
-        <v>1.20444</v>
-      </c>
       <c r="C80">
         <v>0.44885999999999998</v>
       </c>
       <c r="D80">
         <v>0.49308000000000002</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80">
+        <v>1.20444</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>0.62356999999999996</v>
       </c>
-      <c r="B81">
-        <v>1.20377</v>
-      </c>
       <c r="C81">
         <v>0.44814999999999999</v>
       </c>
       <c r="D81">
         <v>0.48571999999999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81">
+        <v>1.20377</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>0.61885000000000001</v>
       </c>
-      <c r="B82">
-        <v>1.2031000000000001</v>
-      </c>
       <c r="C82">
         <v>0.44141999999999998</v>
       </c>
       <c r="D82">
         <v>0.45912999999999998</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82">
+        <v>1.2031000000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>0.61470999999999998</v>
       </c>
-      <c r="B83">
-        <v>1.20242</v>
-      </c>
       <c r="C83">
         <v>0.44418000000000002</v>
       </c>
       <c r="D83">
         <v>0.44529999999999997</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83">
+        <v>1.20242</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>0.60540000000000005</v>
       </c>
-      <c r="B84">
-        <v>1.20174</v>
-      </c>
       <c r="C84">
         <v>0.43164999999999998</v>
       </c>
       <c r="D84">
         <v>0.43774000000000002</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84">
+        <v>1.20174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>0.58589999999999998</v>
       </c>
-      <c r="B85">
-        <v>1.2010400000000001</v>
-      </c>
       <c r="C85">
         <v>0.4158</v>
       </c>
       <c r="D85">
         <v>0.42914999999999998</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85">
+        <v>1.2010400000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>0.57554000000000005</v>
       </c>
-      <c r="B86">
-        <v>1.20034</v>
-      </c>
       <c r="C86">
         <v>0.41432000000000002</v>
       </c>
       <c r="D86">
         <v>0.43347999999999998</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86">
+        <v>1.20034</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>0.58003000000000005</v>
       </c>
-      <c r="B87">
-        <v>1.19964</v>
-      </c>
       <c r="C87">
         <v>0.41360999999999998</v>
       </c>
       <c r="D87">
         <v>0.42430000000000001</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87">
+        <v>1.19964</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>0.59414</v>
       </c>
-      <c r="B88">
-        <v>1.1989399999999999</v>
-      </c>
       <c r="C88">
         <v>0.41425000000000001</v>
       </c>
       <c r="D88">
         <v>0.43492999999999998</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88">
+        <v>1.1989399999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>0.58672000000000002</v>
       </c>
-      <c r="B89">
-        <v>1.19825</v>
-      </c>
       <c r="C89">
         <v>0.40318999999999999</v>
       </c>
       <c r="D89">
         <v>0.42354000000000003</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89">
+        <v>1.19825</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>0.56840000000000002</v>
       </c>
-      <c r="B90">
-        <v>1.19756</v>
-      </c>
       <c r="C90">
         <v>0.39633000000000002</v>
       </c>
       <c r="D90">
         <v>0.41489999999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90">
+        <v>1.19756</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>0.55964000000000003</v>
       </c>
-      <c r="B91">
-        <v>1.1968700000000001</v>
-      </c>
       <c r="C91">
         <v>0.38988</v>
       </c>
       <c r="D91">
         <v>0.41060000000000002</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91">
+        <v>1.1968700000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>0.55367999999999995</v>
       </c>
-      <c r="B92">
-        <v>1.1961900000000001</v>
-      </c>
       <c r="C92">
         <v>0.39842</v>
       </c>
       <c r="D92">
         <v>0.41025</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92">
+        <v>1.1961900000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>0.55037000000000003</v>
       </c>
-      <c r="B93">
-        <v>1.1955199999999999</v>
-      </c>
       <c r="C93">
         <v>0.38323000000000002</v>
       </c>
       <c r="D93">
         <v>0.41682999999999998</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93">
+        <v>1.1955199999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>0.54627000000000003</v>
       </c>
-      <c r="B94">
-        <v>1.19486</v>
-      </c>
       <c r="C94">
         <v>0.38762000000000002</v>
       </c>
       <c r="D94">
         <v>0.38552999999999998</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94">
+        <v>1.19486</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>0.54215000000000002</v>
       </c>
-      <c r="B95">
-        <v>1.1941999999999999</v>
-      </c>
       <c r="C95">
         <v>0.37907999999999997</v>
       </c>
       <c r="D95">
         <v>0.38585000000000003</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95">
+        <v>1.1941999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>0.53695999999999999</v>
       </c>
-      <c r="B96">
-        <v>1.19356</v>
-      </c>
       <c r="C96">
         <v>0.37003000000000003</v>
       </c>
       <c r="D96">
         <v>0.38717000000000001</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96">
+        <v>1.19356</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>0.52939000000000003</v>
       </c>
-      <c r="B97">
-        <v>1.19292</v>
-      </c>
       <c r="C97">
         <v>0.36486000000000002</v>
       </c>
       <c r="D97">
         <v>0.37884000000000001</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97">
+        <v>1.19292</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>0.52663000000000004</v>
       </c>
@@ -8714,7 +8810,7 @@
         <v>0.36810999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>0.51566999999999996</v>
       </c>
@@ -8725,7 +8821,7 @@
         <v>0.36287999999999998</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>0.51349</v>
       </c>
@@ -8736,7 +8832,7 @@
         <v>0.36048999999999998</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>0.49807000000000001</v>
       </c>
@@ -8747,7 +8843,7 @@
         <v>0.3669</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>0.49478</v>
       </c>
@@ -8758,7 +8854,7 @@
         <v>0.34415000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>0.48609000000000002</v>
       </c>
@@ -8769,7 +8865,7 @@
         <v>0.34428999999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>0.49109999999999998</v>
       </c>
@@ -8780,7 +8876,7 @@
         <v>0.34982000000000002</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>0.48444999999999999</v>
       </c>
@@ -8791,7 +8887,7 @@
         <v>0.34572000000000003</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>0.47420000000000001</v>
       </c>
@@ -8802,7 +8898,7 @@
         <v>0.33648</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>0.47017999999999999</v>
       </c>
@@ -8813,7 +8909,7 @@
         <v>0.32311000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>0.46390999999999999</v>
       </c>
@@ -8824,7 +8920,7 @@
         <v>0.32171</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>0.47032000000000002</v>
       </c>
@@ -8835,7 +8931,7 @@
         <v>0.32001000000000002</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>0.45624999999999999</v>
       </c>
@@ -8846,7 +8942,7 @@
         <v>0.30098000000000003</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>0.44896000000000003</v>
       </c>
@@ -8857,7 +8953,7 @@
         <v>0.29605999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>0.44874000000000003</v>
       </c>

</xml_diff>

<commit_message>
NN uploaded, adagrad finished
</commit_message>
<xml_diff>
--- a/Models/TrainingError.xlsx
+++ b/Models/TrainingError.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\514\ImgSegNN\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F571DA-BF7B-4843-A449-2E5E0FA6DD29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F82FD66-41BA-4621-9358-598BA9CAFFB2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NN041201</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +47,10 @@
   </si>
   <si>
     <t>NN041402</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NN041501</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5383,6 +5387,818 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-1ABE-480A-9FED-90AF9A844567}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NN041501</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$513</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="512"/>
+                <c:pt idx="0">
+                  <c:v>2.30599</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.46272</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3350599999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2908200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2646299999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2462200000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2311700000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2180899999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2065399999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.19621</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1869000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.17818</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1701299999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.16275</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1559699999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1496299999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.14374</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.13832</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1332899999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1286099999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.12422</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.12008</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1161700000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.1124099999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.1088100000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.10534</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.1019699999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.0987</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.09544</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.09226</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0891</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.08599</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.08291</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.07986</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0768500000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.0738300000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.07081</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.0678000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0647800000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.0617799999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.05871</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0549900000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.0515399999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.04834</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.04518</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.04203</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.03891</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.0358000000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.0326200000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.02918</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.02596</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.02278</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.01959</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.01641</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.0132099999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.0099899999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.0067600000000001</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.00352</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.0002599999999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.99702999999999997</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.99375999999999998</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.99048999999999998</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.98716000000000004</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.98375999999999997</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.98021000000000003</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.97677000000000003</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.97328999999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.96984000000000004</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.96641999999999995</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.96301999999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.95960999999999996</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.95620000000000005</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.95279000000000003</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.94938999999999996</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.94599</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.94254000000000004</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.93908999999999998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.93564000000000003</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.93218999999999996</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.92856000000000005</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.92496</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.92135999999999996</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.91773000000000005</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.91405999999999998</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.91047999999999996</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.90683999999999998</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.90322000000000002</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.89966999999999997</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.89614000000000005</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89263999999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.88919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.88571</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.88229000000000002</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.87887999999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.87546000000000002</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.87207999999999997</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.86926000000000003</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.86670999999999998</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.86336000000000002</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.86077999999999999</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.85994000000000004</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.85757000000000005</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.86043000000000003</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.86950000000000005</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.87638000000000005</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.87222999999999995</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.86689000000000005</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.85804000000000002</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.84963999999999995</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.84289999999999998</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.83869000000000005</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.83701000000000003</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.83909</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.83935999999999999</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.84277000000000002</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.83904000000000001</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.85743000000000003</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.86573999999999995</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.85258</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.84231999999999996</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.83406000000000002</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.82852999999999999</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.82123999999999997</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.82833999999999997</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.82135000000000002</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.81681000000000004</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.81601000000000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.82311999999999996</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.81657999999999997</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.82149000000000005</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.83540000000000003</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.84416000000000002</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.83274000000000004</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.81962999999999997</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.80949000000000004</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.79984999999999995</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.79993000000000003</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.80113999999999996</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.79676000000000002</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.79410999999999998</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.78771999999999998</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.79752999999999996</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.79556000000000004</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.79842999999999997</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.81416999999999995</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.82487999999999995</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.82128999999999996</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.81572999999999996</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.80500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.79237999999999997</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.78751000000000004</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.78115000000000001</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.78827000000000003</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.78649000000000002</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.78088999999999997</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.77698999999999996</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.78622999999999998</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.80396999999999996</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.81691000000000003</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.81113999999999997</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.79454999999999998</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.77942</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.76549</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.75734999999999997</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.75366</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.75095999999999996</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.74782000000000004</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.74883</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.73992999999999998</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.73945000000000005</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.73831000000000002</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.73860000000000003</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.74448999999999999</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.73782000000000003</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.74309999999999998</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.75180000000000002</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.78634999999999999</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.80135999999999996</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.78881999999999997</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.77288000000000001</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.75773000000000001</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.74763000000000002</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.73882999999999999</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.73633999999999999</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.73165000000000002</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.73589000000000004</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.72821999999999998</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.73309000000000002</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.72802</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.72974000000000006</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.73209999999999997</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.75055000000000005</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.78698000000000001</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.77359</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.75322</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.73314000000000001</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.71940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.71026</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.71031999999999995</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.70660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.70996999999999999</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.70370999999999995</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.70409999999999995</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.70086999999999999</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.70760999999999996</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.71286000000000005</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.70401000000000002</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.70357999999999998</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.70657000000000003</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.71133000000000002</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.72902</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.74695999999999996</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.75007999999999997</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.73807</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.71233999999999997</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.69760999999999995</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.69294999999999995</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.69530999999999998</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.68459000000000003</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.68754000000000004</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.68622000000000005</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.68147000000000002</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.66976000000000002</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.67376000000000003</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.68093999999999999</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.66654999999999998</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.66503999999999996</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.67837000000000003</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.67551000000000005</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.67139000000000004</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.66718999999999995</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.67025000000000001</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.67418999999999996</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.68684999999999996</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.70298000000000005</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.73690999999999995</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.73109999999999997</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.70372999999999997</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.67754999999999999</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.65913999999999995</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.65425999999999995</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.65612000000000004</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.66015999999999997</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.66012000000000004</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.65134000000000003</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.64149</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.64356000000000002</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.64159999999999995</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.63892000000000004</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.64859999999999995</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>0.64698</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>0.64588999999999996</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.65403</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.67178000000000004</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.69860999999999995</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.69111</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9041-42A2-8CF7-822D0A30421B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6271,16 +7087,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6571,10 +7387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F513"/>
+  <dimension ref="A1:G513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6585,9 +7401,10 @@
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="20.25" customWidth="1"/>
     <col min="6" max="6" width="23.125" customWidth="1"/>
+    <col min="7" max="7" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6606,8 +7423,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.40707</v>
       </c>
@@ -6626,8 +7446,11 @@
       <c r="F2">
         <v>2.8994399999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>2.30599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.21393</v>
       </c>
@@ -6646,8 +7469,11 @@
       <c r="F3">
         <v>2.8929100000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>1.46272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1.1911499999999999</v>
       </c>
@@ -6666,8 +7492,11 @@
       <c r="F4">
         <v>2.8862199999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>1.3350599999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1.17875</v>
       </c>
@@ -6686,8 +7515,11 @@
       <c r="F5">
         <v>2.8793600000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>1.2908200000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1.1663399999999999</v>
       </c>
@@ -6706,8 +7538,11 @@
       <c r="F6">
         <v>2.8723000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>1.2646299999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.1603300000000001</v>
       </c>
@@ -6726,8 +7561,11 @@
       <c r="F7">
         <v>2.8650500000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>1.2462200000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1.15283</v>
       </c>
@@ -6746,8 +7584,11 @@
       <c r="F8">
         <v>2.85758</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>1.2311700000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1.14449</v>
       </c>
@@ -6766,8 +7607,11 @@
       <c r="F9">
         <v>2.8498999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>1.2180899999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1.1368499999999999</v>
       </c>
@@ -6786,8 +7630,11 @@
       <c r="F10">
         <v>2.8420000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>1.2065399999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1.1312500000000001</v>
       </c>
@@ -6806,8 +7653,11 @@
       <c r="F11">
         <v>2.83385</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>1.19621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1.12487</v>
       </c>
@@ -6826,8 +7676,11 @@
       <c r="F12">
         <v>2.8254600000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>1.1869000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1.11836</v>
       </c>
@@ -6846,8 +7699,11 @@
       <c r="F13">
         <v>2.8168099999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>1.17818</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1.1136999999999999</v>
       </c>
@@ -6866,8 +7722,11 @@
       <c r="F14">
         <v>2.80789</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>1.1701299999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1.10816</v>
       </c>
@@ -6886,8 +7745,11 @@
       <c r="F15">
         <v>2.79867</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>1.16275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1.1029500000000001</v>
       </c>
@@ -6906,8 +7768,11 @@
       <c r="F16">
         <v>2.7891499999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>1.1559699999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1.0970599999999999</v>
       </c>
@@ -6926,8 +7791,11 @@
       <c r="F17">
         <v>2.7793100000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>1.1496299999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1.09259</v>
       </c>
@@ -6946,8 +7814,11 @@
       <c r="F18">
         <v>2.7691300000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>1.14374</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1.0862099999999999</v>
       </c>
@@ -6966,8 +7837,11 @@
       <c r="F19">
         <v>2.7585899999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>1.13832</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1.0807500000000001</v>
       </c>
@@ -6986,8 +7860,11 @@
       <c r="F20">
         <v>2.7476699999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>1.1332899999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1.0752299999999999</v>
       </c>
@@ -7006,8 +7883,11 @@
       <c r="F21">
         <v>2.7363499999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>1.1286099999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1.06873</v>
       </c>
@@ -7026,8 +7906,11 @@
       <c r="F22">
         <v>2.7246100000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>1.12422</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1.0640000000000001</v>
       </c>
@@ -7046,8 +7929,11 @@
       <c r="F23">
         <v>2.7124199999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>1.12008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1.05697</v>
       </c>
@@ -7066,8 +7952,11 @@
       <c r="F24">
         <v>2.6997599999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>1.1161700000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1.0506</v>
       </c>
@@ -7086,8 +7975,11 @@
       <c r="F25">
         <v>2.6865999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>1.1124099999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1.0446500000000001</v>
       </c>
@@ -7106,8 +7998,11 @@
       <c r="F26">
         <v>2.67292</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>1.1088100000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1.0374099999999999</v>
       </c>
@@ -7126,8 +8021,11 @@
       <c r="F27">
         <v>2.6586699999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>1.10534</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1.0299199999999999</v>
       </c>
@@ -7146,8 +8044,11 @@
       <c r="F28">
         <v>2.6438299999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>1.1019699999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1.02234</v>
       </c>
@@ -7166,8 +8067,11 @@
       <c r="F29">
         <v>2.6283699999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>1.0987</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1.0116099999999999</v>
       </c>
@@ -7186,8 +8090,11 @@
       <c r="F30">
         <v>2.61225</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>1.09544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1.00186</v>
       </c>
@@ -7206,8 +8113,11 @@
       <c r="F31">
         <v>2.5954199999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>1.09226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.99263000000000001</v>
       </c>
@@ -7226,8 +8136,11 @@
       <c r="F32">
         <v>2.5778699999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>1.0891</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.98448999999999998</v>
       </c>
@@ -7246,8 +8159,11 @@
       <c r="F33">
         <v>2.5595300000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>1.08599</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.97646999999999995</v>
       </c>
@@ -7266,8 +8182,11 @@
       <c r="F34">
         <v>2.5403799999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>1.08291</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.96584000000000003</v>
       </c>
@@ -7286,8 +8205,11 @@
       <c r="F35">
         <v>2.5203600000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>1.07986</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.95508000000000004</v>
       </c>
@@ -7306,8 +8228,11 @@
       <c r="F36">
         <v>2.4994399999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>1.0768500000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.94486999999999999</v>
       </c>
@@ -7326,8 +8251,11 @@
       <c r="F37">
         <v>2.4775800000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>1.0738300000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.93822000000000005</v>
       </c>
@@ -7346,8 +8274,11 @@
       <c r="F38">
         <v>2.45472</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>1.07081</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.92762999999999995</v>
       </c>
@@ -7366,8 +8297,11 @@
       <c r="F39">
         <v>2.4308399999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>1.0678000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.92034000000000005</v>
       </c>
@@ -7386,8 +8320,11 @@
       <c r="F40">
         <v>2.4058899999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>1.0647800000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0.91352</v>
       </c>
@@ -7406,8 +8343,11 @@
       <c r="F41">
         <v>2.3798699999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>1.0617799999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0.90368999999999999</v>
       </c>
@@ -7426,8 +8366,11 @@
       <c r="F42">
         <v>2.3527399999999998</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>1.05871</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0.89685000000000004</v>
       </c>
@@ -7446,8 +8389,11 @@
       <c r="F43">
         <v>2.3245</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>1.0549900000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0.89124000000000003</v>
       </c>
@@ -7466,8 +8412,11 @@
       <c r="F44">
         <v>2.29514</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>1.0515399999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0.88793</v>
       </c>
@@ -7486,8 +8435,11 @@
       <c r="F45">
         <v>2.2646700000000002</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>1.04834</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>0.87975000000000003</v>
       </c>
@@ -7506,8 +8458,11 @@
       <c r="F46">
         <v>2.2331099999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>1.04518</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>0.87073</v>
       </c>
@@ -7526,8 +8481,11 @@
       <c r="F47">
         <v>2.20051</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>1.04203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>0.86189000000000004</v>
       </c>
@@ -7546,8 +8504,11 @@
       <c r="F48">
         <v>2.1669100000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>1.03891</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>0.85167000000000004</v>
       </c>
@@ -7566,8 +8527,11 @@
       <c r="F49">
         <v>2.13239</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>1.0358000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>0.84370000000000001</v>
       </c>
@@ -7586,8 +8550,11 @@
       <c r="F50">
         <v>2.0970599999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>1.0326200000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>0.83496000000000004</v>
       </c>
@@ -7606,8 +8573,11 @@
       <c r="F51">
         <v>2.06101</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>1.02918</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>0.82221999999999995</v>
       </c>
@@ -7626,8 +8596,11 @@
       <c r="F52">
         <v>2.0244</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>1.02596</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>0.81574000000000002</v>
       </c>
@@ -7646,8 +8619,11 @@
       <c r="F53">
         <v>1.9873700000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>1.02278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>0.80500000000000005</v>
       </c>
@@ -7666,8 +8642,11 @@
       <c r="F54">
         <v>1.9500999999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>1.01959</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>0.79525000000000001</v>
       </c>
@@ -7686,8 +8665,11 @@
       <c r="F55">
         <v>1.91279</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>1.01641</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>0.78539000000000003</v>
       </c>
@@ -7706,8 +8688,11 @@
       <c r="F56">
         <v>1.8756600000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>1.0132099999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>0.78113999999999995</v>
       </c>
@@ -7726,8 +8711,11 @@
       <c r="F57">
         <v>1.83894</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>1.0099899999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>0.78739000000000003</v>
       </c>
@@ -7746,8 +8734,11 @@
       <c r="F58">
         <v>1.80287</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>1.0067600000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>0.77329000000000003</v>
       </c>
@@ -7766,8 +8757,11 @@
       <c r="F59">
         <v>1.7677</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>1.00352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>0.76321000000000006</v>
       </c>
@@ -7786,8 +8780,11 @@
       <c r="F60">
         <v>1.73367</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>1.0002599999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>0.75377000000000005</v>
       </c>
@@ -7806,8 +8803,11 @@
       <c r="F61">
         <v>1.70103</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>0.99702999999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>0.75034999999999996</v>
       </c>
@@ -7826,8 +8826,11 @@
       <c r="F62">
         <v>1.6699900000000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>0.99375999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>0.74243000000000003</v>
       </c>
@@ -7846,8 +8849,11 @@
       <c r="F63">
         <v>1.6407</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>0.99048999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>0.73775000000000002</v>
       </c>
@@ -7866,8 +8872,11 @@
       <c r="F64">
         <v>1.6133</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>0.98716000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>0.72572000000000003</v>
       </c>
@@ -7886,8 +8895,11 @@
       <c r="F65">
         <v>1.58788</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>0.98375999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>0.71723999999999999</v>
       </c>
@@ -7906,8 +8918,11 @@
       <c r="F66">
         <v>1.5644800000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>0.98021000000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>0.71008000000000004</v>
       </c>
@@ -7926,8 +8941,11 @@
       <c r="F67">
         <v>1.54311</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>0.97677000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>0.71574000000000004</v>
       </c>
@@ -7946,8 +8964,11 @@
       <c r="F68">
         <v>1.52373</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>0.97328999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>0.69894999999999996</v>
       </c>
@@ -7966,8 +8987,11 @@
       <c r="F69">
         <v>1.5062899999999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>0.96984000000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>0.68415000000000004</v>
       </c>
@@ -7986,8 +9010,11 @@
       <c r="F70">
         <v>1.49068</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>0.96641999999999995</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>0.67340999999999995</v>
       </c>
@@ -8006,8 +9033,11 @@
       <c r="F71">
         <v>1.47679</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>0.96301999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>0.66666999999999998</v>
       </c>
@@ -8026,8 +9056,11 @@
       <c r="F72">
         <v>1.46448</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>0.95960999999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>0.66208</v>
       </c>
@@ -8046,8 +9079,11 @@
       <c r="F73">
         <v>1.4536199999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>0.95620000000000005</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>0.66693999999999998</v>
       </c>
@@ -8066,8 +9102,11 @@
       <c r="F74">
         <v>1.4440500000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>0.95279000000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>0.67162999999999995</v>
       </c>
@@ -8086,8 +9125,11 @@
       <c r="F75">
         <v>1.4356500000000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>0.94938999999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>0.65447999999999995</v>
       </c>
@@ -8106,8 +9148,11 @@
       <c r="F76">
         <v>1.42828</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>0.94599</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>0.64273999999999998</v>
       </c>
@@ -8126,8 +9171,11 @@
       <c r="F77">
         <v>1.4218</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>0.94254000000000004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>0.64258999999999999</v>
       </c>
@@ -8146,8 +9194,11 @@
       <c r="F78">
         <v>1.41611</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78">
+        <v>0.93908999999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>0.63590999999999998</v>
       </c>
@@ -8166,8 +9217,11 @@
       <c r="F79">
         <v>1.41109</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79">
+        <v>0.93564000000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>0.62336000000000003</v>
       </c>
@@ -8186,8 +9240,11 @@
       <c r="F80">
         <v>1.4066700000000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <v>0.93218999999999996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>0.62356999999999996</v>
       </c>
@@ -8206,8 +9263,11 @@
       <c r="F81">
         <v>1.4027499999999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81">
+        <v>0.92856000000000005</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>0.61885000000000001</v>
       </c>
@@ -8226,8 +9286,11 @@
       <c r="F82">
         <v>1.3992599999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <v>0.92496</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>0.61470999999999998</v>
       </c>
@@ -8246,8 +9309,11 @@
       <c r="F83">
         <v>1.39615</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83">
+        <v>0.92135999999999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>0.60540000000000005</v>
       </c>
@@ -8266,8 +9332,11 @@
       <c r="F84">
         <v>1.3933599999999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84">
+        <v>0.91773000000000005</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>0.58589999999999998</v>
       </c>
@@ -8286,8 +9355,11 @@
       <c r="F85">
         <v>1.3908400000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85">
+        <v>0.91405999999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>0.57554000000000005</v>
       </c>
@@ -8306,8 +9378,11 @@
       <c r="F86">
         <v>1.38856</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86">
+        <v>0.91047999999999996</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>0.58003000000000005</v>
       </c>
@@ -8326,8 +9401,11 @@
       <c r="F87">
         <v>1.3864799999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87">
+        <v>0.90683999999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>0.59414</v>
       </c>
@@ -8346,8 +9424,11 @@
       <c r="F88">
         <v>1.38456</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88">
+        <v>0.90322000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>0.58672000000000002</v>
       </c>
@@ -8366,8 +9447,11 @@
       <c r="F89">
         <v>1.3828</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89">
+        <v>0.89966999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>0.56840000000000002</v>
       </c>
@@ -8386,8 +9470,11 @@
       <c r="F90">
         <v>1.3811599999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90">
+        <v>0.89614000000000005</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>0.55964000000000003</v>
       </c>
@@ -8406,8 +9493,11 @@
       <c r="F91">
         <v>1.37964</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91">
+        <v>0.89263999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>0.55367999999999995</v>
       </c>
@@ -8426,8 +9516,11 @@
       <c r="F92">
         <v>1.3782000000000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92">
+        <v>0.88919999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>0.55037000000000003</v>
       </c>
@@ -8446,8 +9539,11 @@
       <c r="F93">
         <v>1.3768499999999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93">
+        <v>0.88571</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>0.54627000000000003</v>
       </c>
@@ -8466,8 +9562,11 @@
       <c r="F94">
         <v>1.37557</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94">
+        <v>0.88229000000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>0.54215000000000002</v>
       </c>
@@ -8486,8 +9585,11 @@
       <c r="F95">
         <v>1.37435</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95">
+        <v>0.87887999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>0.53695999999999999</v>
       </c>
@@ -8506,8 +9608,11 @@
       <c r="F96">
         <v>1.3731899999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G96">
+        <v>0.87546000000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>0.52939000000000003</v>
       </c>
@@ -8526,8 +9631,11 @@
       <c r="F97">
         <v>1.3720699999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97">
+        <v>0.87207999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>0.52663000000000004</v>
       </c>
@@ -8546,8 +9654,11 @@
       <c r="F98">
         <v>1.371</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G98">
+        <v>0.86926000000000003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>0.51566999999999996</v>
       </c>
@@ -8566,8 +9677,11 @@
       <c r="F99">
         <v>1.3699600000000001</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G99">
+        <v>0.86670999999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>0.51349</v>
       </c>
@@ -8586,8 +9700,11 @@
       <c r="F100">
         <v>1.3689499999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G100">
+        <v>0.86336000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>0.49807000000000001</v>
       </c>
@@ -8606,8 +9723,11 @@
       <c r="F101">
         <v>1.36798</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G101">
+        <v>0.86077999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>0.49478</v>
       </c>
@@ -8626,8 +9746,11 @@
       <c r="F102">
         <v>1.3670199999999999</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G102">
+        <v>0.85994000000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>0.48609000000000002</v>
       </c>
@@ -8646,8 +9769,11 @@
       <c r="F103">
         <v>1.3661000000000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G103">
+        <v>0.85757000000000005</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>0.49109999999999998</v>
       </c>
@@ -8666,8 +9792,11 @@
       <c r="F104">
         <v>1.3651899999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G104">
+        <v>0.86043000000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>0.48444999999999999</v>
       </c>
@@ -8686,8 +9815,11 @@
       <c r="F105">
         <v>1.3643000000000001</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G105">
+        <v>0.86950000000000005</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>0.47420000000000001</v>
       </c>
@@ -8706,8 +9838,11 @@
       <c r="F106">
         <v>1.3634299999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G106">
+        <v>0.87638000000000005</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>0.47017999999999999</v>
       </c>
@@ -8726,8 +9861,11 @@
       <c r="F107">
         <v>1.3625799999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G107">
+        <v>0.87222999999999995</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>0.46390999999999999</v>
       </c>
@@ -8746,8 +9884,11 @@
       <c r="F108">
         <v>1.36174</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G108">
+        <v>0.86689000000000005</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>0.47032000000000002</v>
       </c>
@@ -8766,8 +9907,11 @@
       <c r="F109">
         <v>1.3609100000000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G109">
+        <v>0.85804000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>0.45624999999999999</v>
       </c>
@@ -8786,8 +9930,11 @@
       <c r="F110">
         <v>1.3601000000000001</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G110">
+        <v>0.84963999999999995</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>0.44896000000000003</v>
       </c>
@@ -8806,8 +9953,11 @@
       <c r="F111">
         <v>1.3593</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G111">
+        <v>0.84289999999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>0.44874000000000003</v>
       </c>
@@ -8826,8 +9976,11 @@
       <c r="F112">
         <v>1.3585100000000001</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G112">
+        <v>0.83869000000000005</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>0.43002000000000001</v>
       </c>
@@ -8846,8 +9999,11 @@
       <c r="F113">
         <v>1.35772</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G113">
+        <v>0.83701000000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>0.41952</v>
       </c>
@@ -8864,8 +10020,11 @@
       <c r="F114">
         <v>1.3569500000000001</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G114">
+        <v>0.83909</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>0.43237999999999999</v>
       </c>
@@ -8882,8 +10041,11 @@
       <c r="F115">
         <v>1.35619</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G115">
+        <v>0.83935999999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>0.41464000000000001</v>
       </c>
@@ -8900,8 +10062,11 @@
       <c r="F116">
         <v>1.3554299999999999</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G116">
+        <v>0.84277000000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>0.41516999999999998</v>
       </c>
@@ -8918,8 +10083,11 @@
       <c r="F117">
         <v>1.3546899999999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G117">
+        <v>0.83904000000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>0.41281000000000001</v>
       </c>
@@ -8936,8 +10104,11 @@
       <c r="F118">
         <v>1.35395</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G118">
+        <v>0.85743000000000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>0.42812</v>
       </c>
@@ -8954,8 +10125,11 @@
       <c r="F119">
         <v>1.3532200000000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G119">
+        <v>0.86573999999999995</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>0.42465000000000003</v>
       </c>
@@ -8972,8 +10146,11 @@
       <c r="F120">
         <v>1.35249</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G120">
+        <v>0.85258</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>0.40384999999999999</v>
       </c>
@@ -8990,8 +10167,11 @@
       <c r="F121">
         <v>1.3517699999999999</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G121">
+        <v>0.84231999999999996</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>0.38895999999999997</v>
       </c>
@@ -9008,8 +10188,11 @@
       <c r="F122">
         <v>1.3510599999999999</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G122">
+        <v>0.83406000000000002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>0.37848999999999999</v>
       </c>
@@ -9026,8 +10209,11 @@
       <c r="F123">
         <v>1.35036</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G123">
+        <v>0.82852999999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>0.37504999999999999</v>
       </c>
@@ -9044,8 +10230,11 @@
       <c r="F124">
         <v>1.3496600000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G124">
+        <v>0.82123999999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>0.37812000000000001</v>
       </c>
@@ -9062,8 +10251,11 @@
       <c r="F125">
         <v>1.3489599999999999</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G125">
+        <v>0.82833999999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>0.36592000000000002</v>
       </c>
@@ -9080,8 +10272,11 @@
       <c r="F126">
         <v>1.3482700000000001</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G126">
+        <v>0.82135000000000002</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>0.35715000000000002</v>
       </c>
@@ -9098,8 +10293,11 @@
       <c r="F127">
         <v>1.3475900000000001</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G127">
+        <v>0.81681000000000004</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>0.35158</v>
       </c>
@@ -9116,8 +10314,11 @@
       <c r="F128">
         <v>1.3469100000000001</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G128">
+        <v>0.81601000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>0.35276999999999997</v>
       </c>
@@ -9134,8 +10335,11 @@
       <c r="F129">
         <v>1.3462400000000001</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G129">
+        <v>0.82311999999999996</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>0.3392</v>
       </c>
@@ -9152,8 +10356,11 @@
       <c r="F130">
         <v>1.3455699999999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G130">
+        <v>0.81657999999999997</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>0.33100000000000002</v>
       </c>
@@ -9170,8 +10377,11 @@
       <c r="F131">
         <v>1.3449</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G131">
+        <v>0.82149000000000005</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>0.33173999999999998</v>
       </c>
@@ -9188,8 +10398,11 @@
       <c r="F132">
         <v>1.3442400000000001</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G132">
+        <v>0.83540000000000003</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>0.32563999999999999</v>
       </c>
@@ -9206,8 +10419,11 @@
       <c r="F133">
         <v>1.3435900000000001</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G133">
+        <v>0.84416000000000002</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>0.32372000000000001</v>
       </c>
@@ -9224,8 +10440,11 @@
       <c r="F134">
         <v>1.34294</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G134">
+        <v>0.83274000000000004</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>0.32943</v>
       </c>
@@ -9242,8 +10461,11 @@
       <c r="F135">
         <v>1.34229</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G135">
+        <v>0.81962999999999997</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>0.33549000000000001</v>
       </c>
@@ -9260,8 +10482,11 @@
       <c r="F136">
         <v>1.34165</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G136">
+        <v>0.80949000000000004</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>0.33040000000000003</v>
       </c>
@@ -9278,8 +10503,11 @@
       <c r="F137">
         <v>1.34101</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G137">
+        <v>0.79984999999999995</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>0.31</v>
       </c>
@@ -9296,8 +10524,11 @@
       <c r="F138">
         <v>1.3403700000000001</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G138">
+        <v>0.79993000000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>0.30270999999999998</v>
       </c>
@@ -9314,8 +10545,11 @@
       <c r="F139">
         <v>1.3397399999999999</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G139">
+        <v>0.80113999999999996</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>0.30506</v>
       </c>
@@ -9332,8 +10566,11 @@
       <c r="F140">
         <v>1.3391200000000001</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G140">
+        <v>0.79676000000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>0.29824000000000001</v>
       </c>
@@ -9350,8 +10587,11 @@
       <c r="F141">
         <v>1.33849</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G141">
+        <v>0.79410999999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>0.29981999999999998</v>
       </c>
@@ -9368,8 +10608,11 @@
       <c r="F142">
         <v>1.3378699999999999</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G142">
+        <v>0.78771999999999998</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>0.29479</v>
       </c>
@@ -9386,8 +10629,11 @@
       <c r="F143">
         <v>1.33725</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G143">
+        <v>0.79752999999999996</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>0.29470000000000002</v>
       </c>
@@ -9404,8 +10650,11 @@
       <c r="F144">
         <v>1.3366400000000001</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G144">
+        <v>0.79556000000000004</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>0.29476999999999998</v>
       </c>
@@ -9422,8 +10671,11 @@
       <c r="F145">
         <v>1.3360300000000001</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G145">
+        <v>0.79842999999999997</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>0.28226000000000001</v>
       </c>
@@ -9440,8 +10692,11 @@
       <c r="F146">
         <v>1.3354200000000001</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G146">
+        <v>0.81416999999999995</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>0.2722</v>
       </c>
@@ -9458,8 +10713,11 @@
       <c r="F147">
         <v>1.3348199999999999</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G147">
+        <v>0.82487999999999995</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>0.26502999999999999</v>
       </c>
@@ -9476,8 +10734,11 @@
       <c r="F148">
         <v>1.33422</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G148">
+        <v>0.82128999999999996</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>0.26445999999999997</v>
       </c>
@@ -9494,8 +10755,11 @@
       <c r="F149">
         <v>1.33362</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G149">
+        <v>0.81572999999999996</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>0.25745000000000001</v>
       </c>
@@ -9512,8 +10776,11 @@
       <c r="F150">
         <v>1.3330299999999999</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G150">
+        <v>0.80500000000000005</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>0.30926999999999999</v>
       </c>
@@ -9530,8 +10797,11 @@
       <c r="F151">
         <v>1.3324400000000001</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G151">
+        <v>0.79237999999999997</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>0.28016999999999997</v>
       </c>
@@ -9548,8 +10818,11 @@
       <c r="F152">
         <v>1.33186</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G152">
+        <v>0.78751000000000004</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>0.25683</v>
       </c>
@@ -9566,8 +10839,11 @@
       <c r="F153">
         <v>1.33128</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G153">
+        <v>0.78115000000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>0.25270999999999999</v>
       </c>
@@ -9584,8 +10860,11 @@
       <c r="F154">
         <v>1.3307</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G154">
+        <v>0.78827000000000003</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>0.25451000000000001</v>
       </c>
@@ -9602,8 +10881,11 @@
       <c r="F155">
         <v>1.33012</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G155">
+        <v>0.78649000000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>0.25818000000000002</v>
       </c>
@@ -9620,8 +10902,11 @@
       <c r="F156">
         <v>1.32955</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G156">
+        <v>0.78088999999999997</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>0.24456</v>
       </c>
@@ -9638,8 +10923,11 @@
       <c r="F157">
         <v>1.3289800000000001</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G157">
+        <v>0.77698999999999996</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>0.24246999999999999</v>
       </c>
@@ -9656,8 +10944,11 @@
       <c r="F158">
         <v>1.3284199999999999</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G158">
+        <v>0.78622999999999998</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>0.24110999999999999</v>
       </c>
@@ -9674,8 +10965,11 @@
       <c r="F159">
         <v>1.32785</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G159">
+        <v>0.80396999999999996</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>0.22721</v>
       </c>
@@ -9692,8 +10986,11 @@
       <c r="F160">
         <v>1.3272900000000001</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G160">
+        <v>0.81691000000000003</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>0.22439000000000001</v>
       </c>
@@ -9710,8 +11007,11 @@
       <c r="F161">
         <v>1.32674</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G161">
+        <v>0.81113999999999997</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>0.21545</v>
       </c>
@@ -9728,8 +11028,11 @@
       <c r="F162">
         <v>1.32619</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G162">
+        <v>0.79454999999999998</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>0.21892</v>
       </c>
@@ -9746,8 +11049,11 @@
       <c r="F163">
         <v>1.3256399999999999</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G163">
+        <v>0.77942</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>0.21693000000000001</v>
       </c>
@@ -9764,8 +11070,11 @@
       <c r="F164">
         <v>1.3250999999999999</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G164">
+        <v>0.76549</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>0.22827</v>
       </c>
@@ -9782,8 +11091,11 @@
       <c r="F165">
         <v>1.32456</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G165">
+        <v>0.75734999999999997</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>0.21335000000000001</v>
       </c>
@@ -9800,8 +11112,11 @@
       <c r="F166">
         <v>1.32403</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G166">
+        <v>0.75366</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>0.21489</v>
       </c>
@@ -9818,8 +11133,11 @@
       <c r="F167">
         <v>1.3234999999999999</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G167">
+        <v>0.75095999999999996</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>0.20755000000000001</v>
       </c>
@@ -9836,8 +11154,11 @@
       <c r="F168">
         <v>1.32298</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G168">
+        <v>0.74782000000000004</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>0.20574999999999999</v>
       </c>
@@ -9854,8 +11175,11 @@
       <c r="F169">
         <v>1.32246</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G169">
+        <v>0.74883</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>0.20321</v>
       </c>
@@ -9872,8 +11196,11 @@
       <c r="F170">
         <v>1.3219399999999999</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G170">
+        <v>0.73992999999999998</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>0.193</v>
       </c>
@@ -9890,8 +11217,11 @@
       <c r="F171">
         <v>1.3214300000000001</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G171">
+        <v>0.73945000000000005</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>0.19892000000000001</v>
       </c>
@@ -9908,8 +11238,11 @@
       <c r="F172">
         <v>1.3209299999999999</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G172">
+        <v>0.73831000000000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>0.19649</v>
       </c>
@@ -9926,8 +11259,11 @@
       <c r="F173">
         <v>1.32043</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G173">
+        <v>0.73860000000000003</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>0.19911999999999999</v>
       </c>
@@ -9944,8 +11280,11 @@
       <c r="F174">
         <v>1.31993</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G174">
+        <v>0.74448999999999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>0.19706000000000001</v>
       </c>
@@ -9962,8 +11301,11 @@
       <c r="F175">
         <v>1.3194399999999999</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G175">
+        <v>0.73782000000000003</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>0.18289</v>
       </c>
@@ -9980,8 +11322,11 @@
       <c r="F176">
         <v>1.3189500000000001</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G176">
+        <v>0.74309999999999998</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>0.17509</v>
       </c>
@@ -9998,8 +11343,11 @@
       <c r="F177">
         <v>1.31846</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G177">
+        <v>0.75180000000000002</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>0.16594</v>
       </c>
@@ -10016,8 +11364,11 @@
       <c r="F178">
         <v>1.3179799999999999</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G178">
+        <v>0.78634999999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>0.16971</v>
       </c>
@@ -10034,8 +11385,11 @@
       <c r="F179">
         <v>1.31751</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G179">
+        <v>0.80135999999999996</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>0.17502999999999999</v>
       </c>
@@ -10052,8 +11406,11 @@
       <c r="F180">
         <v>1.31704</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G180">
+        <v>0.78881999999999997</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>0.19539999999999999</v>
       </c>
@@ -10070,8 +11427,11 @@
       <c r="F181">
         <v>1.31657</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G181">
+        <v>0.77288000000000001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>0.17637</v>
       </c>
@@ -10088,8 +11448,11 @@
       <c r="F182">
         <v>1.3161099999999999</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G182">
+        <v>0.75773000000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>0.16108</v>
       </c>
@@ -10106,8 +11469,11 @@
       <c r="F183">
         <v>1.31565</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G183">
+        <v>0.74763000000000002</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>0.16381000000000001</v>
       </c>
@@ -10124,8 +11490,11 @@
       <c r="F184">
         <v>1.3151900000000001</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G184">
+        <v>0.73882999999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>0.15601999999999999</v>
       </c>
@@ -10142,8 +11511,11 @@
       <c r="F185">
         <v>1.31474</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G185">
+        <v>0.73633999999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>0.15185999999999999</v>
       </c>
@@ -10160,8 +11532,11 @@
       <c r="F186">
         <v>1.3143</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G186">
+        <v>0.73165000000000002</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>0.15282000000000001</v>
       </c>
@@ -10178,8 +11553,11 @@
       <c r="F187">
         <v>1.31386</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G187">
+        <v>0.73589000000000004</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>0.15049999999999999</v>
       </c>
@@ -10196,8 +11574,11 @@
       <c r="F188">
         <v>1.31342</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G188">
+        <v>0.72821999999999998</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>0.15559999999999999</v>
       </c>
@@ -10214,8 +11595,11 @@
       <c r="F189">
         <v>1.3129900000000001</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G189">
+        <v>0.73309000000000002</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>0.15060000000000001</v>
       </c>
@@ -10232,8 +11616,11 @@
       <c r="F190">
         <v>1.31257</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G190">
+        <v>0.72802</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>0.15193000000000001</v>
       </c>
@@ -10250,8 +11637,11 @@
       <c r="F191">
         <v>1.3121400000000001</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G191">
+        <v>0.72974000000000006</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>0.17412</v>
       </c>
@@ -10268,8 +11658,11 @@
       <c r="F192">
         <v>1.3117300000000001</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G192">
+        <v>0.73209999999999997</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>0.15371000000000001</v>
       </c>
@@ -10286,8 +11679,11 @@
       <c r="F193">
         <v>1.31131</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G193">
+        <v>0.75055000000000005</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>0.14726</v>
       </c>
@@ -10304,8 +11700,11 @@
       <c r="F194">
         <v>1.3109</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G194">
+        <v>0.78698000000000001</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>0.14654</v>
       </c>
@@ -10322,8 +11721,11 @@
       <c r="F195">
         <v>1.3105</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G195">
+        <v>0.77359</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>0.14136000000000001</v>
       </c>
@@ -10340,8 +11742,11 @@
       <c r="F196">
         <v>1.3101</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G196">
+        <v>0.75322</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>0.13678999999999999</v>
       </c>
@@ -10358,8 +11763,11 @@
       <c r="F197">
         <v>1.3097000000000001</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G197">
+        <v>0.73314000000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>0.14480000000000001</v>
       </c>
@@ -10376,8 +11784,11 @@
       <c r="F198">
         <v>1.30931</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G198">
+        <v>0.71940999999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>0.13808000000000001</v>
       </c>
@@ -10394,8 +11805,11 @@
       <c r="F199">
         <v>1.3089299999999999</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G199">
+        <v>0.71026</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>0.14410000000000001</v>
       </c>
@@ -10412,8 +11826,11 @@
       <c r="F200">
         <v>1.30854</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G200">
+        <v>0.71031999999999995</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>0.13768</v>
       </c>
@@ -10430,8 +11847,11 @@
       <c r="F201">
         <v>1.3081700000000001</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G201">
+        <v>0.70660000000000001</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>0.14094999999999999</v>
       </c>
@@ -10448,8 +11868,11 @@
       <c r="F202">
         <v>1.30779</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G202">
+        <v>0.70996999999999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>0.14656</v>
       </c>
@@ -10466,8 +11889,11 @@
       <c r="F203">
         <v>1.30742</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G203">
+        <v>0.70370999999999995</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>0.14285999999999999</v>
       </c>
@@ -10484,8 +11910,11 @@
       <c r="F204">
         <v>1.3070600000000001</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G204">
+        <v>0.70409999999999995</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>0.12920999999999999</v>
       </c>
@@ -10502,8 +11931,11 @@
       <c r="F205">
         <v>1.3067</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G205">
+        <v>0.70086999999999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>0.12268</v>
       </c>
@@ -10520,8 +11952,11 @@
       <c r="F206">
         <v>1.3063400000000001</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G206">
+        <v>0.70760999999999996</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>0.12182</v>
       </c>
@@ -10538,8 +11973,11 @@
       <c r="F207">
         <v>1.30599</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G207">
+        <v>0.71286000000000005</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>0.12303</v>
       </c>
@@ -10556,8 +11994,11 @@
       <c r="F208">
         <v>1.3056399999999999</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G208">
+        <v>0.70401000000000002</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>0.11706</v>
       </c>
@@ -10574,8 +12015,11 @@
       <c r="F209">
         <v>1.3052900000000001</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G209">
+        <v>0.70357999999999998</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>0.11583</v>
       </c>
@@ -10592,8 +12036,11 @@
       <c r="F210">
         <v>1.3049500000000001</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G210">
+        <v>0.70657000000000003</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>0.11219999999999999</v>
       </c>
@@ -10610,8 +12057,11 @@
       <c r="F211">
         <v>1.30461</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G211">
+        <v>0.71133000000000002</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>0.11840000000000001</v>
       </c>
@@ -10628,8 +12078,11 @@
       <c r="F212">
         <v>1.30427</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G212">
+        <v>0.72902</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>0.12573999999999999</v>
       </c>
@@ -10646,8 +12099,11 @@
       <c r="F213">
         <v>1.3039400000000001</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G213">
+        <v>0.74695999999999996</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>0.11380999999999999</v>
       </c>
@@ -10664,8 +12120,11 @@
       <c r="F214">
         <v>1.3036099999999999</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G214">
+        <v>0.75007999999999997</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>0.11224000000000001</v>
       </c>
@@ -10682,8 +12141,11 @@
       <c r="F215">
         <v>1.30328</v>
       </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G215">
+        <v>0.73807</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>0.11314</v>
       </c>
@@ -10700,8 +12162,11 @@
       <c r="F216">
         <v>1.3029599999999999</v>
       </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G216">
+        <v>0.71233999999999997</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>0.12751999999999999</v>
       </c>
@@ -10718,8 +12183,11 @@
       <c r="F217">
         <v>1.30264</v>
       </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G217">
+        <v>0.69760999999999995</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>0.13441</v>
       </c>
@@ -10736,8 +12204,11 @@
       <c r="F218">
         <v>1.30233</v>
       </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G218">
+        <v>0.69294999999999995</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>0.11197</v>
       </c>
@@ -10754,8 +12225,11 @@
       <c r="F219">
         <v>1.30202</v>
       </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G219">
+        <v>0.69530999999999998</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>0.11214</v>
       </c>
@@ -10772,8 +12246,11 @@
       <c r="F220">
         <v>1.3017099999999999</v>
       </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G220">
+        <v>0.68459000000000003</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>0.10238</v>
       </c>
@@ -10790,8 +12267,11 @@
       <c r="F221">
         <v>1.3013999999999999</v>
       </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G221">
+        <v>0.68754000000000004</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>9.9419999999999994E-2</v>
       </c>
@@ -10808,8 +12288,11 @@
       <c r="F222">
         <v>1.3010999999999999</v>
       </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G222">
+        <v>0.68622000000000005</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>9.7000000000000003E-2</v>
       </c>
@@ -10826,8 +12309,11 @@
       <c r="F223">
         <v>1.3008</v>
       </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G223">
+        <v>0.68147000000000002</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>0.10054</v>
       </c>
@@ -10844,8 +12330,11 @@
       <c r="F224">
         <v>1.3005100000000001</v>
       </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G224">
+        <v>0.66976000000000002</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>0.10248</v>
       </c>
@@ -10862,8 +12351,11 @@
       <c r="F225">
         <v>1.3002199999999999</v>
       </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G225">
+        <v>0.67376000000000003</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>0.10149</v>
       </c>
@@ -10880,8 +12372,11 @@
       <c r="F226">
         <v>1.29993</v>
       </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G226">
+        <v>0.68093999999999999</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>0.10385</v>
       </c>
@@ -10898,8 +12393,11 @@
       <c r="F227">
         <v>1.2996399999999999</v>
       </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G227">
+        <v>0.66654999999999998</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>0.10721</v>
       </c>
@@ -10916,8 +12414,11 @@
       <c r="F228">
         <v>1.2993600000000001</v>
       </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G228">
+        <v>0.66503999999999996</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>0.10183</v>
       </c>
@@ -10934,8 +12435,11 @@
       <c r="F229">
         <v>1.29908</v>
       </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G229">
+        <v>0.67837000000000003</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>9.8419999999999994E-2</v>
       </c>
@@ -10952,8 +12456,11 @@
       <c r="F230">
         <v>1.2988</v>
       </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G230">
+        <v>0.67551000000000005</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>9.9959999999999993E-2</v>
       </c>
@@ -10970,8 +12477,11 @@
       <c r="F231">
         <v>1.29853</v>
       </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G231">
+        <v>0.67139000000000004</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>9.8540000000000003E-2</v>
       </c>
@@ -10988,8 +12498,11 @@
       <c r="F232">
         <v>1.2982499999999999</v>
       </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G232">
+        <v>0.66718999999999995</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>9.2439999999999994E-2</v>
       </c>
@@ -11006,8 +12519,11 @@
       <c r="F233">
         <v>1.2979799999999999</v>
       </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G233">
+        <v>0.67025000000000001</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>9.4060000000000005E-2</v>
       </c>
@@ -11024,8 +12540,11 @@
       <c r="F234">
         <v>1.29772</v>
       </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G234">
+        <v>0.67418999999999996</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>8.8090000000000002E-2</v>
       </c>
@@ -11042,8 +12561,11 @@
       <c r="F235">
         <v>1.29745</v>
       </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G235">
+        <v>0.68684999999999996</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>0.11858</v>
       </c>
@@ -11060,8 +12582,11 @@
       <c r="F236">
         <v>1.2971900000000001</v>
       </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G236">
+        <v>0.70298000000000005</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>9.1450000000000004E-2</v>
       </c>
@@ -11078,8 +12603,11 @@
       <c r="F237">
         <v>1.2969299999999999</v>
       </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G237">
+        <v>0.73690999999999995</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>8.6099999999999996E-2</v>
       </c>
@@ -11096,8 +12624,11 @@
       <c r="F238">
         <v>1.29667</v>
       </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G238">
+        <v>0.73109999999999997</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>8.5680000000000006E-2</v>
       </c>
@@ -11114,8 +12645,11 @@
       <c r="F239">
         <v>1.2964199999999999</v>
       </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G239">
+        <v>0.70372999999999997</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>9.7239999999999993E-2</v>
       </c>
@@ -11132,8 +12666,11 @@
       <c r="F240">
         <v>1.29616</v>
       </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G240">
+        <v>0.67754999999999999</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>0.1134</v>
       </c>
@@ -11150,8 +12687,11 @@
       <c r="F241">
         <v>1.2959099999999999</v>
       </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G241">
+        <v>0.65913999999999995</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>0.10904999999999999</v>
       </c>
@@ -11168,8 +12708,11 @@
       <c r="F242">
         <v>1.2956700000000001</v>
       </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G242">
+        <v>0.65425999999999995</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>9.1689999999999994E-2</v>
       </c>
@@ -11186,8 +12729,11 @@
       <c r="F243">
         <v>1.29542</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G243">
+        <v>0.65612000000000004</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>8.881E-2</v>
       </c>
@@ -11204,8 +12750,11 @@
       <c r="F244">
         <v>1.29518</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G244">
+        <v>0.66015999999999997</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>8.4110000000000004E-2</v>
       </c>
@@ -11222,8 +12771,11 @@
       <c r="F245">
         <v>1.2949299999999999</v>
       </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G245">
+        <v>0.66012000000000004</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>7.911E-2</v>
       </c>
@@ -11240,8 +12792,11 @@
       <c r="F246">
         <v>1.2947</v>
       </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G246">
+        <v>0.65134000000000003</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>0.10452</v>
       </c>
@@ -11258,8 +12813,11 @@
       <c r="F247">
         <v>1.2944599999999999</v>
       </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G247">
+        <v>0.64149</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>9.06E-2</v>
       </c>
@@ -11276,8 +12834,11 @@
       <c r="F248">
         <v>1.2942199999999999</v>
       </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G248">
+        <v>0.64356000000000002</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>8.6139999999999994E-2</v>
       </c>
@@ -11294,8 +12855,11 @@
       <c r="F249">
         <v>1.29399</v>
       </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G249">
+        <v>0.64159999999999995</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>7.7630000000000005E-2</v>
       </c>
@@ -11312,8 +12876,11 @@
       <c r="F250">
         <v>1.29376</v>
       </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G250">
+        <v>0.63892000000000004</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>7.4359999999999996E-2</v>
       </c>
@@ -11330,8 +12897,11 @@
       <c r="F251">
         <v>1.2935300000000001</v>
       </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G251">
+        <v>0.64859999999999995</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>7.8549999999999995E-2</v>
       </c>
@@ -11348,8 +12918,11 @@
       <c r="F252">
         <v>1.2932999999999999</v>
       </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G252">
+        <v>0.64698</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>7.8770000000000007E-2</v>
       </c>
@@ -11366,8 +12939,11 @@
       <c r="F253">
         <v>1.2930699999999999</v>
       </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G253">
+        <v>0.64588999999999996</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>7.5389999999999999E-2</v>
       </c>
@@ -11384,8 +12960,11 @@
       <c r="F254">
         <v>1.2928500000000001</v>
       </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G254">
+        <v>0.65403</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>7.4520000000000003E-2</v>
       </c>
@@ -11402,8 +12981,11 @@
       <c r="F255">
         <v>1.2926299999999999</v>
       </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G255">
+        <v>0.67178000000000004</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>7.3510000000000006E-2</v>
       </c>
@@ -11420,8 +13002,11 @@
       <c r="F256">
         <v>1.2924100000000001</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G256">
+        <v>0.69860999999999995</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>7.9289999999999999E-2</v>
       </c>
@@ -11438,92 +13023,95 @@
       <c r="F257">
         <v>1.2921899999999999</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G257">
+        <v>0.69111</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>8.5059999999999997E-2</v>
       </c>
       <c r="B258" s="1"/>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>9.8199999999999996E-2</v>
       </c>
       <c r="B259" s="1"/>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>8.6790000000000006E-2</v>
       </c>
       <c r="B260" s="1"/>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>7.8560000000000005E-2</v>
       </c>
       <c r="B261" s="1"/>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>7.1669999999999998E-2</v>
       </c>
       <c r="B262" s="1"/>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>6.769E-2</v>
       </c>
       <c r="B263" s="1"/>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>6.5659999999999996E-2</v>
       </c>
       <c r="B264" s="1"/>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>8.8220000000000007E-2</v>
       </c>
       <c r="B265" s="1"/>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>8.5180000000000006E-2</v>
       </c>
       <c r="B266" s="1"/>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>9.4990000000000005E-2</v>
       </c>
       <c r="B267" s="1"/>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>7.46E-2</v>
       </c>
       <c r="B268" s="1"/>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>7.3810000000000001E-2</v>
       </c>
       <c r="B269" s="1"/>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>6.3439999999999996E-2</v>
       </c>
       <c r="B270" s="1"/>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>6.1249999999999999E-2</v>
       </c>
       <c r="B271" s="1"/>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>6.3619999999999996E-2</v>
       </c>

</xml_diff>

<commit_message>
learning rate scheduler fixed
</commit_message>
<xml_diff>
--- a/Models/TrainingError.xlsx
+++ b/Models/TrainingError.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\514\ImgSegNN\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFAEED5-5395-4DD6-8210-1C6CE88450B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF15A266-C8E1-4686-BAFA-1C4102110A87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ConvergePatternOfNN" sheetId="1" r:id="rId1"/>
+    <sheet name="LearningRateScheduler" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>NN041201</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +56,14 @@
   </si>
   <si>
     <t>NN041502</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power=1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -203,7 +212,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>ConvergePatternOfNN!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -226,7 +235,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$257</c:f>
+              <c:f>ConvergePatternOfNN!$B$2:$B$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -1013,7 +1022,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>ConvergePatternOfNN!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1036,7 +1045,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$257</c:f>
+              <c:f>ConvergePatternOfNN!$C$2:$C$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -1823,7 +1832,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>ConvergePatternOfNN!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1846,7 +1855,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$257</c:f>
+              <c:f>ConvergePatternOfNN!$D$2:$D$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -2633,7 +2642,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>ConvergePatternOfNN!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2656,7 +2665,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$257</c:f>
+              <c:f>ConvergePatternOfNN!$E$2:$E$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -3443,7 +3452,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>ConvergePatternOfNN!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3466,7 +3475,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$257</c:f>
+              <c:f>ConvergePatternOfNN!$F$2:$F$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -4253,7 +4262,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>ConvergePatternOfNN!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4276,7 +4285,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$257</c:f>
+              <c:f>ConvergePatternOfNN!$G$2:$G$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -5063,7 +5072,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>ConvergePatternOfNN!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5088,7 +5097,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$257</c:f>
+              <c:f>ConvergePatternOfNN!$H$2:$H$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -6195,6 +6204,2009 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>PolynomialLRDecay</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LearningRateScheduler!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power=2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>LearningRateScheduler!$A$2:$A$257</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="256"/>
+                <c:pt idx="0">
+                  <c:v>9.9228073120117104E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9228073120117104E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8459167480468707E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7693283081054603E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6930419921875E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6170578002929604E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5413757324218692E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4659957885742194E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3909179687500007E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.3161422729492096E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.2416687011718703E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.1674972534179604E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.0936279296875006E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.0200607299804596E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.9467956542968706E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.8738327026367195E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.8011718749999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.7288131713867192E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.65675659179687E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.5850021362304692E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.5135498046874994E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.4423995971679693E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.3715515136718703E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.3010055541992093E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.2307617187500001E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.1608200073242099E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.0911804199218697E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.0218429565429693E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.9528076171875E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.88407440185546E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.8156433105468701E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.7475143432617199E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.6796874999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.6121627807617196E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.5449401855468704E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.47801971435546E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4114013671874998E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.3450851440429697E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.2790710449218698E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.2133590698242097E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.1479492187499997E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.0828414916992198E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.0180358886718702E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.9535324096679698E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.8893310546874996E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.82543182373047E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.7618347167968697E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.69853973388671E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6.6355468750000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.5728561401367097E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6.51046752929687E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.4483810424804597E-3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.3865966796875003E-3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.3251144409179599E-3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.2639343261718704E-3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.2030563354492198E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.1424804687500003E-3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6.0822067260742196E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6.0222351074218699E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.96256561279296E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.9031982421875002E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.8441329956054697E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.7853698730468703E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.7269088745117097E-3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.6687500000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.6108932495117104E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.5533386230468698E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.4960861206054604E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.4391357421875001E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.3824874877929597E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5.3261413574218703E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.2700973510742197E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.2143554687500001E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.1589157104492099E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.1037780761718698E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.0489425659179599E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.9944091796875001E-3</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.9401779174804697E-3</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.8862487792968702E-3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.8326217651367097E-3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.7792968750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.7262741088867103E-3</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.6735534667968698E-3</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.6211349487304603E-3</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.5690185546875001E-3</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.5172042846679597E-3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.4656921386718703E-3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.4144821166992197E-3</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.3635742187500002E-3</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.3129684448242099E-3</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.2626647949218699E-3</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.21266326904296E-3</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4.1629638671875002E-3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.1135665893554697E-3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.0644714355468703E-3</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4.0156784057617098E-3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.9671875000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.9189987182617096E-3</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.8711120605468699E-3</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.82352752685546E-3</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3.7762451171874998E-3</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3.7292648315429599E-3</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3.68258666992187E-3</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3.6362106323242099E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3.5901367187499999E-3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3.5443649291992101E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3.4988952636718701E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3.4537277221679602E-3</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3.4088623046875E-3</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3.36429901123046E-3</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3.3200378417968701E-3</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.27607879638671E-3</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3.2324218750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3.1890670776367099E-3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>3.1460144042968702E-3</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>3.1032638549804599E-3</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3.0608154296875001E-3</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>3.0186691284179602E-3</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2.9768249511718699E-3</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>2.9352828979492102E-3</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2.8940429687499998E-3</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2.85310516357421E-3</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2.81246948242187E-3</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2.7721359252929601E-3</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2.7321044921874999E-3</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2.6923751831054599E-3</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2.6529479980468701E-3</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2.61382293701171E-3</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2.575E-3</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>2.5364791870117098E-3</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2.4982604980468702E-3</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2.4603439331054599E-3</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2.4227294921875002E-3</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2.3854171752929602E-3</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>2.3484069824218699E-3</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.3116989135742098E-3</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2.2752929687499999E-3</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2.2391891479492101E-3</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2.2033874511718701E-3</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2.1678878784179602E-3</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2.1326904296875E-3</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2.09779510498046E-3</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2.0632019042968702E-3</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2.0289108276367101E-3</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1.9949218750000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1.96123504638671E-3</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1.9278503417968699E-3</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1.8947677612304601E-3</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.8619873046874999E-3</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.8295089721679599E-3</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.7973327636718701E-3</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1.76545867919921E-3</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1.7338867187500001E-3</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1.7026168823242099E-3</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1.6716491699218701E-3</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1.64098358154296E-3</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1.6106201171875E-3</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>1.5805587768554601E-3</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1.55079956054687E-3</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1.52134246826171E-3</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1.4921875E-3</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1.4633346557617101E-3</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>1.43478393554687E-3</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1.40653533935546E-3</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1.3785888671875E-3</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1.3509445190429601E-3</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1.32360229492187E-3</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1.29656219482421E-3</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1.26982421875E-3</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1.2433883666992101E-3</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1.21725463867187E-3</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1.19142303466796E-3</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>1.1658935546875E-3</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1.1406661987304601E-3</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>1.11574096679687E-3</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1.09111785888671E-3</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>1.066796875E-3</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1.0427780151367101E-3</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1.0190612792968701E-3</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>9.9564666748046802E-4</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>9.7253417968749996E-4</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>9.4972381591796804E-4</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>9.2721557617187497E-4</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>9.0500946044921795E-4</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>8.8310546874999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>8.6150360107421797E-4</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>8.4020385742187502E-4</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>8.1920623779296799E-4</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>7.9851074218750004E-4</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>7.7811737060546802E-4</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>7.5802612304687496E-4</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>7.3823699951171805E-4</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>7.1874999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>6.9956512451171797E-4</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>6.8068237304687502E-4</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>6.62101745605468E-4</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>6.4382324218750005E-4</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>6.2584686279296804E-4</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>6.0817260742187498E-4</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>5.9080047607421797E-4</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>5.7373046875000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>5.5696258544921801E-4</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>5.4049682617187495E-4</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>5.2433319091796805E-4</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>5.084716796875E-4</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>4.9291229248046799E-4</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>4.7765502929687499E-4</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>4.6269989013671798E-4</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>4.4804687499999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>4.3369598388671798E-4</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>4.1964721679687498E-4</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>4.0590057373046797E-4</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>3.9245605468749998E-4</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>3.7931365966796797E-4</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>3.6647338867187498E-4</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>3.5393524169921798E-4</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>3.4169921874999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>3.2976531982421798E-4</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3.18133544921875E-4</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>3.0680389404296799E-4</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>2.9577636718750001E-4</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2.85050964355468E-4</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>2.7462768554687502E-4</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>2.6450653076171801E-4</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>2.5468749999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>2.4517059326171798E-4</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2.3595581054687499E-4</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>2.2704315185546799E-4</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>2.1843261718750001E-4</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2.1012420654296799E-4</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2.0211791992187501E-4</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1.9441375732421801E-4</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>1.8701171875E-4</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>1.7991180419921801E-4</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1.73114013671875E-4</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1.6661834716796801E-4</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>1.604248046875E-4</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>1.5453338623046801E-4</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1.4894409179687501E-4</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1.4365692138671799E-4</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1.3867187499999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1.33988952636718E-4</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1.29608154296875E-4</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1.2552947998046801E-4</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1.2175292968749999E-4</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1.1827850341796801E-4</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1.1510620117187499E-4</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1.1223602294921799E-4</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1.0966796875E-4</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1.07402038574218E-4</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1.05438232421875E-4</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1.03776550292968E-4</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1.024169921875E-4</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1.01359558105468E-4</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1.0060424804687501E-4</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1.00151062011718E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99AA-4CD9-B92D-88D585553266}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LearningRateScheduler!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power=1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>LearningRateScheduler!$B$2:$B$257</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="256"/>
+                <c:pt idx="0">
+                  <c:v>9.9613281250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9613281250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9226562500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.883984375E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8453124999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8066406249999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.7679687499999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.7292968749999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6906249999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.6519531249999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6132812499999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.5746093749999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.5359374999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.4972656249999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.4585937500000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.4199218750000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.3812500000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.3425781250000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.3039062500000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.2652343750000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.2265625000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.1878906250000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.1492187500000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1105468750000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.0718750000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.033203125E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.9945312499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.9558593749999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.9171874999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.8785156249999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.8398437499999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.8011718749999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.7624999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.7238281249999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.6851562499999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.6464843749999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.6078124999999991E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8.5691406250000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.5304687500000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.4917968750000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.4531250000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.4144531250000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8.3757812500000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8.3371093750000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.2984375000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.2597656250000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.2210937500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.182421875E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8.1437499999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.1050781249999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>8.0664062499999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.0277343749999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7.9890624999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7.9503906249999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7.9117187499999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>7.8730468749999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7.8343749999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7.7957031250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.75703125E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7.718359375E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.6796874999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.6410156249999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>7.6023437499999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.5636718749999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7.5249999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7.4863281250000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.4476562500000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>7.4089843750000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7.3703125000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7.331640625E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7.29296875E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.2542968749999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.2156249999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.1769531249999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.1382812499999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.0996093749999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.0609375000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.0222656250000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.9835937500000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.9449218750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.9062500000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.867578125E-3</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.8289062499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.7902343749999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.7515624999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.7128906249999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6.6742187499999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6.6355468750000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6.5968750000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.5582031250000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.5195312500000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.4808593750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.4421875E-3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6.4035156249999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6.3648437499999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>6.3261718749999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6.2874999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>6.2488281249999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.2101562500000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.1714843750000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.1328125000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>6.0941406250000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>6.0554687500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>6.016796875E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>5.9781249999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>5.9394531249999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>5.9007812499999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>5.8621093749999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>5.8234374999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>5.7847656250000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>5.7460937500000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>5.7074218750000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>5.6687500000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>5.6300781250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>5.59140625E-3</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>5.5527343749999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>5.5140624999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>5.4753906249999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>5.4367187499999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>5.3980468749999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>5.3593750000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>5.3207031250000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>5.2820312500000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.2433593750000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>5.2046875000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>5.166015625E-3</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>5.12734375E-3</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>5.0886718749999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>5.0499999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>5.0113281249999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>4.9726562499999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>4.9339843749999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>4.8953125000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>4.8566406250000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>4.8179687500000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>4.7792968750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>4.740625E-3</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>4.701953125E-3</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>4.6632812499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>4.6246093749999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>4.5859374999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>4.5472656249999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>4.5085937499999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>4.4699218750000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.4312500000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>4.3925781250000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4.3539062500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>4.3152343750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>4.2765625E-3</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4.2378906249999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>4.1992187499999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>4.1605468749999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>4.1218749999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>4.0832031249999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>4.0445312500000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>4.0058593750000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>3.9671875000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>3.9285156250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>3.8898437500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>3.851171875E-3</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>3.8124999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>3.7738281249999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>3.7351562500000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>3.6964843750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>3.6578125E-3</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>3.619140625E-3</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>3.5804687499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>3.5417968749999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>3.5031250000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>3.4644531250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>3.42578125E-3</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>3.3871093749999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>3.3484374999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>3.3097656250000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>3.2710937500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>3.2324218750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>3.19375E-3</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>3.1550781249999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>3.1164062499999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>3.0777343750000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>3.0390625000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>3.000390625E-3</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>2.9617187499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2.9230468749999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2.8843749999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>2.8457031250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2.8070312500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>2.768359375E-3</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2.7296874999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>2.6910156249999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>2.6523437500000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2.6136718750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>2.575E-3</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2.536328125E-3</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2.4976562499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2.4589843749999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>2.4203125000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>2.3816406250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2.34296875E-3</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>2.3042968749999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>2.2656249999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2.2269531250000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>2.1882812500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2.149609375E-3</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>2.1109375E-3</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2.0722656249999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2.0335937499999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1.9949218750000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1.9562500000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1.917578125E-3</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1.8789062499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1.8402343750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1.8015625E-3</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1.7628906249999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>1.7242187500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>1.685546875E-3</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1.6468749999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>1.608203125E-3</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1.56953125E-3</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>1.5308593750000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>1.4921875E-3</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>1.4535156249999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>1.4148437500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>1.376171875E-3</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>1.3374999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>1.2988281250000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>1.26015625E-3</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>1.2214843749999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1.1828125000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1.144140625E-3</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>1.1054687499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1.066796875E-3</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>1.028125E-3</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>9.894531250000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>9.5078125000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>9.1210937500000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>8.7343749999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>8.34765625E-4</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>7.9609375000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>7.5742187499999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>7.1874999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>6.8007812500000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>6.4140625000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>6.0273437499999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>5.640625E-4</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>5.2539062500000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>4.8671875000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>4.4804687499999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>4.0937500000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>3.7070312499999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>3.3203125000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>2.93359375E-4</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>2.5468749999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>2.1601562500000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1.7734375000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1.3867187499999999E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-99AA-4CD9-B92D-88D585553266}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="335908895"/>
+        <c:axId val="2133561007"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="335908895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Number of epochs</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2133561007"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2133561007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Learning Rate</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="335908895"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6235,7 +8247,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6792,6 +9360,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEF729B9-18D5-4B4A-B2C3-193047254AB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7057,7 +9666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -15056,4 +17665,2077 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443D35BB-E572-41C3-9409-E11A3769A3F0}">
+  <dimension ref="A1:B257"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A241" sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>9.9228073120117104E-3</v>
+      </c>
+      <c r="B2">
+        <v>9.9613281250000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>9.9228073120117104E-3</v>
+      </c>
+      <c r="B3">
+        <v>9.9613281250000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>9.8459167480468707E-3</v>
+      </c>
+      <c r="B4">
+        <v>9.9226562500000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>9.7693283081054603E-3</v>
+      </c>
+      <c r="B5">
+        <v>9.883984375E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>9.6930419921875E-3</v>
+      </c>
+      <c r="B6">
+        <v>9.8453124999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>9.6170578002929604E-3</v>
+      </c>
+      <c r="B7">
+        <v>9.8066406249999998E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>9.5413757324218692E-3</v>
+      </c>
+      <c r="B8">
+        <v>9.7679687499999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9.4659957885742194E-3</v>
+      </c>
+      <c r="B9">
+        <v>9.7292968749999997E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9.3909179687500007E-3</v>
+      </c>
+      <c r="B10">
+        <v>9.6906249999999996E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9.3161422729492096E-3</v>
+      </c>
+      <c r="B11">
+        <v>9.6519531249999995E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9.2416687011718703E-3</v>
+      </c>
+      <c r="B12">
+        <v>9.6132812499999994E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9.1674972534179604E-3</v>
+      </c>
+      <c r="B13">
+        <v>9.5746093749999994E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>9.0936279296875006E-3</v>
+      </c>
+      <c r="B14">
+        <v>9.5359374999999993E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>9.0200607299804596E-3</v>
+      </c>
+      <c r="B15">
+        <v>9.4972656249999992E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>8.9467956542968706E-3</v>
+      </c>
+      <c r="B16">
+        <v>9.4585937500000009E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8.8738327026367195E-3</v>
+      </c>
+      <c r="B17">
+        <v>9.4199218750000008E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8.8011718749999995E-3</v>
+      </c>
+      <c r="B18">
+        <v>9.3812500000000007E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>8.7288131713867192E-3</v>
+      </c>
+      <c r="B19">
+        <v>9.3425781250000006E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>8.65675659179687E-3</v>
+      </c>
+      <c r="B20">
+        <v>9.3039062500000005E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>8.5850021362304692E-3</v>
+      </c>
+      <c r="B21">
+        <v>9.2652343750000005E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>8.5135498046874994E-3</v>
+      </c>
+      <c r="B22">
+        <v>9.2265625000000004E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8.4423995971679693E-3</v>
+      </c>
+      <c r="B23">
+        <v>9.1878906250000003E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>8.3715515136718703E-3</v>
+      </c>
+      <c r="B24">
+        <v>9.1492187500000002E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8.3010055541992093E-3</v>
+      </c>
+      <c r="B25">
+        <v>9.1105468750000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>8.2307617187500001E-3</v>
+      </c>
+      <c r="B26">
+        <v>9.0718750000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>8.1608200073242099E-3</v>
+      </c>
+      <c r="B27">
+        <v>9.033203125E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>8.0911804199218697E-3</v>
+      </c>
+      <c r="B28">
+        <v>8.9945312499999999E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>8.0218429565429693E-3</v>
+      </c>
+      <c r="B29">
+        <v>8.9558593749999998E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>7.9528076171875E-3</v>
+      </c>
+      <c r="B30">
+        <v>8.9171874999999998E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>7.88407440185546E-3</v>
+      </c>
+      <c r="B31">
+        <v>8.8785156249999997E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>7.8156433105468701E-3</v>
+      </c>
+      <c r="B32">
+        <v>8.8398437499999996E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>7.7475143432617199E-3</v>
+      </c>
+      <c r="B33">
+        <v>8.8011718749999995E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>7.6796874999999999E-3</v>
+      </c>
+      <c r="B34">
+        <v>8.7624999999999995E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>7.6121627807617196E-3</v>
+      </c>
+      <c r="B35">
+        <v>8.7238281249999994E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>7.5449401855468704E-3</v>
+      </c>
+      <c r="B36">
+        <v>8.6851562499999993E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>7.47801971435546E-3</v>
+      </c>
+      <c r="B37">
+        <v>8.6464843749999992E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>7.4114013671874998E-3</v>
+      </c>
+      <c r="B38">
+        <v>8.6078124999999991E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>7.3450851440429697E-3</v>
+      </c>
+      <c r="B39">
+        <v>8.5691406250000008E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>7.2790710449218698E-3</v>
+      </c>
+      <c r="B40">
+        <v>8.5304687500000007E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7.2133590698242097E-3</v>
+      </c>
+      <c r="B41">
+        <v>8.4917968750000006E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>7.1479492187499997E-3</v>
+      </c>
+      <c r="B42">
+        <v>8.4531250000000006E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7.0828414916992198E-3</v>
+      </c>
+      <c r="B43">
+        <v>8.4144531250000005E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>7.0180358886718702E-3</v>
+      </c>
+      <c r="B44">
+        <v>8.3757812500000004E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>6.9535324096679698E-3</v>
+      </c>
+      <c r="B45">
+        <v>8.3371093750000003E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>6.8893310546874996E-3</v>
+      </c>
+      <c r="B46">
+        <v>8.2984375000000003E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>6.82543182373047E-3</v>
+      </c>
+      <c r="B47">
+        <v>8.2597656250000002E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>6.7618347167968697E-3</v>
+      </c>
+      <c r="B48">
+        <v>8.2210937500000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>6.69853973388671E-3</v>
+      </c>
+      <c r="B49">
+        <v>8.182421875E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>6.6355468750000004E-3</v>
+      </c>
+      <c r="B50">
+        <v>8.1437499999999999E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>6.5728561401367097E-3</v>
+      </c>
+      <c r="B51">
+        <v>8.1050781249999999E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>6.51046752929687E-3</v>
+      </c>
+      <c r="B52">
+        <v>8.0664062499999998E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>6.4483810424804597E-3</v>
+      </c>
+      <c r="B53">
+        <v>8.0277343749999997E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>6.3865966796875003E-3</v>
+      </c>
+      <c r="B54">
+        <v>7.9890624999999996E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>6.3251144409179599E-3</v>
+      </c>
+      <c r="B55">
+        <v>7.9503906249999996E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>6.2639343261718704E-3</v>
+      </c>
+      <c r="B56">
+        <v>7.9117187499999995E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>6.2030563354492198E-3</v>
+      </c>
+      <c r="B57">
+        <v>7.8730468749999994E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>6.1424804687500003E-3</v>
+      </c>
+      <c r="B58">
+        <v>7.8343749999999993E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>6.0822067260742196E-3</v>
+      </c>
+      <c r="B59">
+        <v>7.7957031250000001E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>6.0222351074218699E-3</v>
+      </c>
+      <c r="B60">
+        <v>7.75703125E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>5.96256561279296E-3</v>
+      </c>
+      <c r="B61">
+        <v>7.718359375E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>5.9031982421875002E-3</v>
+      </c>
+      <c r="B62">
+        <v>7.6796874999999999E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>5.8441329956054697E-3</v>
+      </c>
+      <c r="B63">
+        <v>7.6410156249999998E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>5.7853698730468703E-3</v>
+      </c>
+      <c r="B64">
+        <v>7.6023437499999997E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>5.7269088745117097E-3</v>
+      </c>
+      <c r="B65">
+        <v>7.5636718749999996E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>5.6687500000000002E-3</v>
+      </c>
+      <c r="B66">
+        <v>7.5249999999999996E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>5.6108932495117104E-3</v>
+      </c>
+      <c r="B67">
+        <v>7.4863281250000004E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>5.5533386230468698E-3</v>
+      </c>
+      <c r="B68">
+        <v>7.4476562500000003E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>5.4960861206054604E-3</v>
+      </c>
+      <c r="B69">
+        <v>7.4089843750000002E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>5.4391357421875001E-3</v>
+      </c>
+      <c r="B70">
+        <v>7.3703125000000001E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>5.3824874877929597E-3</v>
+      </c>
+      <c r="B71">
+        <v>7.331640625E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>5.3261413574218703E-3</v>
+      </c>
+      <c r="B72">
+        <v>7.29296875E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>5.2700973510742197E-3</v>
+      </c>
+      <c r="B73">
+        <v>7.2542968749999999E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>5.2143554687500001E-3</v>
+      </c>
+      <c r="B74">
+        <v>7.2156249999999998E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>5.1589157104492099E-3</v>
+      </c>
+      <c r="B75">
+        <v>7.1769531249999997E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>5.1037780761718698E-3</v>
+      </c>
+      <c r="B76">
+        <v>7.1382812499999997E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>5.0489425659179599E-3</v>
+      </c>
+      <c r="B77">
+        <v>7.0996093749999996E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>4.9944091796875001E-3</v>
+      </c>
+      <c r="B78">
+        <v>7.0609375000000004E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>4.9401779174804697E-3</v>
+      </c>
+      <c r="B79">
+        <v>7.0222656250000003E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>4.8862487792968702E-3</v>
+      </c>
+      <c r="B80">
+        <v>6.9835937500000002E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>4.8326217651367097E-3</v>
+      </c>
+      <c r="B81">
+        <v>6.9449218750000001E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>4.7792968750000001E-3</v>
+      </c>
+      <c r="B82">
+        <v>6.9062500000000001E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>4.7262741088867103E-3</v>
+      </c>
+      <c r="B83">
+        <v>6.867578125E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>4.6735534667968698E-3</v>
+      </c>
+      <c r="B84">
+        <v>6.8289062499999999E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>4.6211349487304603E-3</v>
+      </c>
+      <c r="B85">
+        <v>6.7902343749999998E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>4.5690185546875001E-3</v>
+      </c>
+      <c r="B86">
+        <v>6.7515624999999998E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>4.5172042846679597E-3</v>
+      </c>
+      <c r="B87">
+        <v>6.7128906249999997E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>4.4656921386718703E-3</v>
+      </c>
+      <c r="B88">
+        <v>6.6742187499999996E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>4.4144821166992197E-3</v>
+      </c>
+      <c r="B89">
+        <v>6.6355468750000004E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>4.3635742187500002E-3</v>
+      </c>
+      <c r="B90">
+        <v>6.5968750000000003E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>4.3129684448242099E-3</v>
+      </c>
+      <c r="B91">
+        <v>6.5582031250000002E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>4.2626647949218699E-3</v>
+      </c>
+      <c r="B92">
+        <v>6.5195312500000002E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>4.21266326904296E-3</v>
+      </c>
+      <c r="B93">
+        <v>6.4808593750000001E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>4.1629638671875002E-3</v>
+      </c>
+      <c r="B94">
+        <v>6.4421875E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>4.1135665893554697E-3</v>
+      </c>
+      <c r="B95">
+        <v>6.4035156249999999E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>4.0644714355468703E-3</v>
+      </c>
+      <c r="B96">
+        <v>6.3648437499999998E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>4.0156784057617098E-3</v>
+      </c>
+      <c r="B97">
+        <v>6.3261718749999998E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>3.9671875000000002E-3</v>
+      </c>
+      <c r="B98">
+        <v>6.2874999999999997E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>3.9189987182617096E-3</v>
+      </c>
+      <c r="B99">
+        <v>6.2488281249999996E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>3.8711120605468699E-3</v>
+      </c>
+      <c r="B100">
+        <v>6.2101562500000004E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>3.82352752685546E-3</v>
+      </c>
+      <c r="B101">
+        <v>6.1714843750000003E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>3.7762451171874998E-3</v>
+      </c>
+      <c r="B102">
+        <v>6.1328125000000002E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>3.7292648315429599E-3</v>
+      </c>
+      <c r="B103">
+        <v>6.0941406250000002E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>3.68258666992187E-3</v>
+      </c>
+      <c r="B104">
+        <v>6.0554687500000001E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>3.6362106323242099E-3</v>
+      </c>
+      <c r="B105">
+        <v>6.016796875E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>3.5901367187499999E-3</v>
+      </c>
+      <c r="B106">
+        <v>5.9781249999999999E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>3.5443649291992101E-3</v>
+      </c>
+      <c r="B107">
+        <v>5.9394531249999999E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>3.4988952636718701E-3</v>
+      </c>
+      <c r="B108">
+        <v>5.9007812499999998E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>3.4537277221679602E-3</v>
+      </c>
+      <c r="B109">
+        <v>5.8621093749999997E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>3.4088623046875E-3</v>
+      </c>
+      <c r="B110">
+        <v>5.8234374999999996E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>3.36429901123046E-3</v>
+      </c>
+      <c r="B111">
+        <v>5.7847656250000004E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>3.3200378417968701E-3</v>
+      </c>
+      <c r="B112">
+        <v>5.7460937500000003E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>3.27607879638671E-3</v>
+      </c>
+      <c r="B113">
+        <v>5.7074218750000003E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>3.2324218750000001E-3</v>
+      </c>
+      <c r="B114">
+        <v>5.6687500000000002E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>3.1890670776367099E-3</v>
+      </c>
+      <c r="B115">
+        <v>5.6300781250000001E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>3.1460144042968702E-3</v>
+      </c>
+      <c r="B116">
+        <v>5.59140625E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>3.1032638549804599E-3</v>
+      </c>
+      <c r="B117">
+        <v>5.5527343749999999E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>3.0608154296875001E-3</v>
+      </c>
+      <c r="B118">
+        <v>5.5140624999999999E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>3.0186691284179602E-3</v>
+      </c>
+      <c r="B119">
+        <v>5.4753906249999998E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>2.9768249511718699E-3</v>
+      </c>
+      <c r="B120">
+        <v>5.4367187499999997E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>2.9352828979492102E-3</v>
+      </c>
+      <c r="B121">
+        <v>5.3980468749999996E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>2.8940429687499998E-3</v>
+      </c>
+      <c r="B122">
+        <v>5.3593750000000004E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>2.85310516357421E-3</v>
+      </c>
+      <c r="B123">
+        <v>5.3207031250000003E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>2.81246948242187E-3</v>
+      </c>
+      <c r="B124">
+        <v>5.2820312500000003E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>2.7721359252929601E-3</v>
+      </c>
+      <c r="B125">
+        <v>5.2433593750000002E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>2.7321044921874999E-3</v>
+      </c>
+      <c r="B126">
+        <v>5.2046875000000001E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>2.6923751831054599E-3</v>
+      </c>
+      <c r="B127">
+        <v>5.166015625E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>2.6529479980468701E-3</v>
+      </c>
+      <c r="B128">
+        <v>5.12734375E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>2.61382293701171E-3</v>
+      </c>
+      <c r="B129">
+        <v>5.0886718749999999E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>2.575E-3</v>
+      </c>
+      <c r="B130">
+        <v>5.0499999999999998E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>2.5364791870117098E-3</v>
+      </c>
+      <c r="B131">
+        <v>5.0113281249999997E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>2.4982604980468702E-3</v>
+      </c>
+      <c r="B132">
+        <v>4.9726562499999996E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>2.4603439331054599E-3</v>
+      </c>
+      <c r="B133">
+        <v>4.9339843749999996E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>2.4227294921875002E-3</v>
+      </c>
+      <c r="B134">
+        <v>4.8953125000000004E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>2.3854171752929602E-3</v>
+      </c>
+      <c r="B135">
+        <v>4.8566406250000003E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>2.3484069824218699E-3</v>
+      </c>
+      <c r="B136">
+        <v>4.8179687500000002E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>2.3116989135742098E-3</v>
+      </c>
+      <c r="B137">
+        <v>4.7792968750000001E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>2.2752929687499999E-3</v>
+      </c>
+      <c r="B138">
+        <v>4.740625E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>2.2391891479492101E-3</v>
+      </c>
+      <c r="B139">
+        <v>4.701953125E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>2.2033874511718701E-3</v>
+      </c>
+      <c r="B140">
+        <v>4.6632812499999999E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>2.1678878784179602E-3</v>
+      </c>
+      <c r="B141">
+        <v>4.6246093749999998E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>2.1326904296875E-3</v>
+      </c>
+      <c r="B142">
+        <v>4.5859374999999997E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>2.09779510498046E-3</v>
+      </c>
+      <c r="B143">
+        <v>4.5472656249999997E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>2.0632019042968702E-3</v>
+      </c>
+      <c r="B144">
+        <v>4.5085937499999996E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>2.0289108276367101E-3</v>
+      </c>
+      <c r="B145">
+        <v>4.4699218750000004E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>1.9949218750000002E-3</v>
+      </c>
+      <c r="B146">
+        <v>4.4312500000000003E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>1.96123504638671E-3</v>
+      </c>
+      <c r="B147">
+        <v>4.3925781250000002E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>1.9278503417968699E-3</v>
+      </c>
+      <c r="B148">
+        <v>4.3539062500000001E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>1.8947677612304601E-3</v>
+      </c>
+      <c r="B149">
+        <v>4.3152343750000001E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>1.8619873046874999E-3</v>
+      </c>
+      <c r="B150">
+        <v>4.2765625E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>1.8295089721679599E-3</v>
+      </c>
+      <c r="B151">
+        <v>4.2378906249999999E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>1.7973327636718701E-3</v>
+      </c>
+      <c r="B152">
+        <v>4.1992187499999998E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>1.76545867919921E-3</v>
+      </c>
+      <c r="B153">
+        <v>4.1605468749999997E-3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>1.7338867187500001E-3</v>
+      </c>
+      <c r="B154">
+        <v>4.1218749999999997E-3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>1.7026168823242099E-3</v>
+      </c>
+      <c r="B155">
+        <v>4.0832031249999996E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>1.6716491699218701E-3</v>
+      </c>
+      <c r="B156">
+        <v>4.0445312500000004E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>1.64098358154296E-3</v>
+      </c>
+      <c r="B157">
+        <v>4.0058593750000003E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>1.6106201171875E-3</v>
+      </c>
+      <c r="B158">
+        <v>3.9671875000000002E-3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>1.5805587768554601E-3</v>
+      </c>
+      <c r="B159">
+        <v>3.9285156250000001E-3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>1.55079956054687E-3</v>
+      </c>
+      <c r="B160">
+        <v>3.8898437500000001E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>1.52134246826171E-3</v>
+      </c>
+      <c r="B161">
+        <v>3.851171875E-3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>1.4921875E-3</v>
+      </c>
+      <c r="B162">
+        <v>3.8124999999999999E-3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>1.4633346557617101E-3</v>
+      </c>
+      <c r="B163">
+        <v>3.7738281249999998E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>1.43478393554687E-3</v>
+      </c>
+      <c r="B164">
+        <v>3.7351562500000002E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>1.40653533935546E-3</v>
+      </c>
+      <c r="B165">
+        <v>3.6964843750000001E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>1.3785888671875E-3</v>
+      </c>
+      <c r="B166">
+        <v>3.6578125E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>1.3509445190429601E-3</v>
+      </c>
+      <c r="B167">
+        <v>3.619140625E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>1.32360229492187E-3</v>
+      </c>
+      <c r="B168">
+        <v>3.5804687499999999E-3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>1.29656219482421E-3</v>
+      </c>
+      <c r="B169">
+        <v>3.5417968749999998E-3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>1.26982421875E-3</v>
+      </c>
+      <c r="B170">
+        <v>3.5031250000000002E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>1.2433883666992101E-3</v>
+      </c>
+      <c r="B171">
+        <v>3.4644531250000001E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>1.21725463867187E-3</v>
+      </c>
+      <c r="B172">
+        <v>3.42578125E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>1.19142303466796E-3</v>
+      </c>
+      <c r="B173">
+        <v>3.3871093749999999E-3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>1.1658935546875E-3</v>
+      </c>
+      <c r="B174">
+        <v>3.3484374999999999E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>1.1406661987304601E-3</v>
+      </c>
+      <c r="B175">
+        <v>3.3097656250000002E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>1.11574096679687E-3</v>
+      </c>
+      <c r="B176">
+        <v>3.2710937500000001E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>1.09111785888671E-3</v>
+      </c>
+      <c r="B177">
+        <v>3.2324218750000001E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>1.066796875E-3</v>
+      </c>
+      <c r="B178">
+        <v>3.19375E-3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>1.0427780151367101E-3</v>
+      </c>
+      <c r="B179">
+        <v>3.1550781249999999E-3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>1.0190612792968701E-3</v>
+      </c>
+      <c r="B180">
+        <v>3.1164062499999998E-3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>9.9564666748046802E-4</v>
+      </c>
+      <c r="B181">
+        <v>3.0777343750000002E-3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>9.7253417968749996E-4</v>
+      </c>
+      <c r="B182">
+        <v>3.0390625000000001E-3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>9.4972381591796804E-4</v>
+      </c>
+      <c r="B183">
+        <v>3.000390625E-3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>9.2721557617187497E-4</v>
+      </c>
+      <c r="B184">
+        <v>2.9617187499999999E-3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>9.0500946044921795E-4</v>
+      </c>
+      <c r="B185">
+        <v>2.9230468749999999E-3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>8.8310546874999999E-4</v>
+      </c>
+      <c r="B186">
+        <v>2.8843749999999998E-3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>8.6150360107421797E-4</v>
+      </c>
+      <c r="B187">
+        <v>2.8457031250000001E-3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>8.4020385742187502E-4</v>
+      </c>
+      <c r="B188">
+        <v>2.8070312500000001E-3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>8.1920623779296799E-4</v>
+      </c>
+      <c r="B189">
+        <v>2.768359375E-3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>7.9851074218750004E-4</v>
+      </c>
+      <c r="B190">
+        <v>2.7296874999999999E-3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>7.7811737060546802E-4</v>
+      </c>
+      <c r="B191">
+        <v>2.6910156249999998E-3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>7.5802612304687496E-4</v>
+      </c>
+      <c r="B192">
+        <v>2.6523437500000002E-3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>7.3823699951171805E-4</v>
+      </c>
+      <c r="B193">
+        <v>2.6136718750000001E-3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>7.1874999999999999E-4</v>
+      </c>
+      <c r="B194">
+        <v>2.575E-3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>6.9956512451171797E-4</v>
+      </c>
+      <c r="B195">
+        <v>2.536328125E-3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>6.8068237304687502E-4</v>
+      </c>
+      <c r="B196">
+        <v>2.4976562499999999E-3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>6.62101745605468E-4</v>
+      </c>
+      <c r="B197">
+        <v>2.4589843749999998E-3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>6.4382324218750005E-4</v>
+      </c>
+      <c r="B198">
+        <v>2.4203125000000002E-3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>6.2584686279296804E-4</v>
+      </c>
+      <c r="B199">
+        <v>2.3816406250000001E-3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>6.0817260742187498E-4</v>
+      </c>
+      <c r="B200">
+        <v>2.34296875E-3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>5.9080047607421797E-4</v>
+      </c>
+      <c r="B201">
+        <v>2.3042968749999999E-3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>5.7373046875000002E-4</v>
+      </c>
+      <c r="B202">
+        <v>2.2656249999999998E-3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>5.5696258544921801E-4</v>
+      </c>
+      <c r="B203">
+        <v>2.2269531250000002E-3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>5.4049682617187495E-4</v>
+      </c>
+      <c r="B204">
+        <v>2.1882812500000001E-3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>5.2433319091796805E-4</v>
+      </c>
+      <c r="B205">
+        <v>2.149609375E-3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>5.084716796875E-4</v>
+      </c>
+      <c r="B206">
+        <v>2.1109375E-3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>4.9291229248046799E-4</v>
+      </c>
+      <c r="B207">
+        <v>2.0722656249999999E-3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>4.7765502929687499E-4</v>
+      </c>
+      <c r="B208">
+        <v>2.0335937499999998E-3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>4.6269989013671798E-4</v>
+      </c>
+      <c r="B209">
+        <v>1.9949218750000002E-3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>4.4804687499999999E-4</v>
+      </c>
+      <c r="B210">
+        <v>1.9562500000000001E-3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>4.3369598388671798E-4</v>
+      </c>
+      <c r="B211">
+        <v>1.917578125E-3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>4.1964721679687498E-4</v>
+      </c>
+      <c r="B212">
+        <v>1.8789062499999999E-3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>4.0590057373046797E-4</v>
+      </c>
+      <c r="B213">
+        <v>1.8402343750000001E-3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>3.9245605468749998E-4</v>
+      </c>
+      <c r="B214">
+        <v>1.8015625E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>3.7931365966796797E-4</v>
+      </c>
+      <c r="B215">
+        <v>1.7628906249999999E-3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>3.6647338867187498E-4</v>
+      </c>
+      <c r="B216">
+        <v>1.7242187500000001E-3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>3.5393524169921798E-4</v>
+      </c>
+      <c r="B217">
+        <v>1.685546875E-3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>3.4169921874999999E-4</v>
+      </c>
+      <c r="B218">
+        <v>1.6468749999999999E-3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>3.2976531982421798E-4</v>
+      </c>
+      <c r="B219">
+        <v>1.608203125E-3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>3.18133544921875E-4</v>
+      </c>
+      <c r="B220">
+        <v>1.56953125E-3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>3.0680389404296799E-4</v>
+      </c>
+      <c r="B221">
+        <v>1.5308593750000001E-3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>2.9577636718750001E-4</v>
+      </c>
+      <c r="B222">
+        <v>1.4921875E-3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>2.85050964355468E-4</v>
+      </c>
+      <c r="B223">
+        <v>1.4535156249999999E-3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>2.7462768554687502E-4</v>
+      </c>
+      <c r="B224">
+        <v>1.4148437500000001E-3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>2.6450653076171801E-4</v>
+      </c>
+      <c r="B225">
+        <v>1.376171875E-3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>2.5468749999999998E-4</v>
+      </c>
+      <c r="B226">
+        <v>1.3374999999999999E-3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>2.4517059326171798E-4</v>
+      </c>
+      <c r="B227">
+        <v>1.2988281250000001E-3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>2.3595581054687499E-4</v>
+      </c>
+      <c r="B228">
+        <v>1.26015625E-3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>2.2704315185546799E-4</v>
+      </c>
+      <c r="B229">
+        <v>1.2214843749999999E-3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>2.1843261718750001E-4</v>
+      </c>
+      <c r="B230">
+        <v>1.1828125000000001E-3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>2.1012420654296799E-4</v>
+      </c>
+      <c r="B231">
+        <v>1.144140625E-3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>2.0211791992187501E-4</v>
+      </c>
+      <c r="B232">
+        <v>1.1054687499999999E-3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>1.9441375732421801E-4</v>
+      </c>
+      <c r="B233">
+        <v>1.066796875E-3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>1.8701171875E-4</v>
+      </c>
+      <c r="B234">
+        <v>1.028125E-3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>1.7991180419921801E-4</v>
+      </c>
+      <c r="B235">
+        <v>9.894531250000001E-4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>1.73114013671875E-4</v>
+      </c>
+      <c r="B236">
+        <v>9.5078125000000002E-4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>1.6661834716796801E-4</v>
+      </c>
+      <c r="B237">
+        <v>9.1210937500000005E-4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>1.604248046875E-4</v>
+      </c>
+      <c r="B238">
+        <v>8.7343749999999997E-4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>1.5453338623046801E-4</v>
+      </c>
+      <c r="B239">
+        <v>8.34765625E-4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>1.4894409179687501E-4</v>
+      </c>
+      <c r="B240">
+        <v>7.9609375000000003E-4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>1.4365692138671799E-4</v>
+      </c>
+      <c r="B241">
+        <v>7.5742187499999996E-4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>1.3867187499999999E-4</v>
+      </c>
+      <c r="B242">
+        <v>7.1874999999999999E-4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>1.33988952636718E-4</v>
+      </c>
+      <c r="B243">
+        <v>6.8007812500000002E-4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>1.29608154296875E-4</v>
+      </c>
+      <c r="B244">
+        <v>6.4140625000000005E-4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>1.2552947998046801E-4</v>
+      </c>
+      <c r="B245">
+        <v>6.0273437499999997E-4</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>1.2175292968749999E-4</v>
+      </c>
+      <c r="B246">
+        <v>5.640625E-4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>1.1827850341796801E-4</v>
+      </c>
+      <c r="B247">
+        <v>5.2539062500000003E-4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>1.1510620117187499E-4</v>
+      </c>
+      <c r="B248">
+        <v>4.8671875000000001E-4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>1.1223602294921799E-4</v>
+      </c>
+      <c r="B249">
+        <v>4.4804687499999999E-4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>1.0966796875E-4</v>
+      </c>
+      <c r="B250">
+        <v>4.0937500000000002E-4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>1.07402038574218E-4</v>
+      </c>
+      <c r="B251">
+        <v>3.7070312499999999E-4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>1.05438232421875E-4</v>
+      </c>
+      <c r="B252">
+        <v>3.3203125000000002E-4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>1.03776550292968E-4</v>
+      </c>
+      <c r="B253">
+        <v>2.93359375E-4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>1.024169921875E-4</v>
+      </c>
+      <c r="B254">
+        <v>2.5468749999999998E-4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>1.01359558105468E-4</v>
+      </c>
+      <c r="B255">
+        <v>2.1601562500000001E-4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>1.0060424804687501E-4</v>
+      </c>
+      <c r="B256">
+        <v>1.7734375000000001E-4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>1.00151062011718E-4</v>
+      </c>
+      <c r="B257">
+        <v>1.3867187499999999E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>